<commit_message>
feat: add package for D2.30
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -16,17 +16,22 @@
     <sheet name="categoryOptionGroupSets" sheetId="11" r:id="rId11"/>
     <sheet name="categoryOptionGroups" sheetId="12" r:id="rId12"/>
     <sheet name="categoryOptionGroupsBySet" sheetId="13" r:id="rId13"/>
-    <sheet name="indicatorGroups" sheetId="14" r:id="rId14"/>
-    <sheet name="indicators" sheetId="15" r:id="rId15"/>
-    <sheet name="indicatorTypes" sheetId="16" r:id="rId16"/>
-    <sheet name="dashboards" sheetId="17" r:id="rId17"/>
-    <sheet name="dashboardItems" sheetId="18" r:id="rId18"/>
-    <sheet name="charts" sheetId="19" r:id="rId19"/>
-    <sheet name="reportTables" sheetId="20" r:id="rId20"/>
-    <sheet name="maps" sheetId="21" r:id="rId21"/>
-    <sheet name="mapViews" sheetId="22" r:id="rId22"/>
-    <sheet name="userGroups" sheetId="23" r:id="rId23"/>
-    <sheet name="users" sheetId="24" r:id="rId24"/>
+    <sheet name="optionSets" sheetId="14" r:id="rId14"/>
+    <sheet name="options" sheetId="15" r:id="rId15"/>
+    <sheet name="validationRules" sheetId="16" r:id="rId16"/>
+    <sheet name="validationRuleGroups" sheetId="17" r:id="rId17"/>
+    <sheet name="validationRules by group" sheetId="18" r:id="rId18"/>
+    <sheet name="indicatorGroups" sheetId="19" r:id="rId19"/>
+    <sheet name="indicators" sheetId="20" r:id="rId20"/>
+    <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
+    <sheet name="dashboards" sheetId="22" r:id="rId22"/>
+    <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
+    <sheet name="maps" sheetId="26" r:id="rId26"/>
+    <sheet name="mapViews" sheetId="27" r:id="rId27"/>
+    <sheet name="userGroups" sheetId="28" r:id="rId28"/>
+    <sheet name="users" sheetId="29" r:id="rId29"/>
   </sheets>
 </workbook>
 </file>
@@ -442,7 +447,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,7 +471,7 @@
         <v>Type</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>AGG</v>
+        <v>COMPLETE</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +479,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COMPLETE</v>
+        <v>V2.0</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +487,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>V1.0.1</v>
+        <v>DHIS2.30</v>
       </c>
     </row>
     <row r="6">
@@ -490,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>DHIS2.30</v>
+        <v>2020-10-12T13:48</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID19_AGG_COMPLETE_V1.0.1_DHIS2.30_2020-03-27T08:26</v>
+        <v>COVID19_COMPLETE_V2.0_DHIS2.30_2020-10-12T13:48</v>
       </c>
     </row>
   </sheetData>
@@ -507,12 +512,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -530,420 +535,497 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years, Female</v>
+        <v>0-4 years, Female</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>h72VZMAIXNp</v>
+        <v>X7SGUlfmJa5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>0-1 years, Male</v>
+        <v>0-4 years, Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>NZkmbtZAFtN</v>
+        <v>d1XzGx028Z8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>0-4 years, Female</v>
+        <v>0-4 years, Unknown Sex</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>JzrkRqzvWhH</v>
+        <v>Ter1Z3EGkQM</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>0-4 years, Male</v>
+        <v>10-14 years, Female</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jQqLIn3xasU</v>
+        <v>vvpjmqp0psR</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>15-24 years, Female</v>
+        <v>10-14 years, Male</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>gPWH4piZwC0</v>
+        <v>SV1RvPdmAkj</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>15-24 years, Male</v>
+        <v>10-14 years, Unknown Sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>uhLnCuMwCGm</v>
+        <v>XUXU9zyHXN9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>15-49 years, Female</v>
+        <v>15-19 years, Female</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>sFJsKLHLBFj</v>
+        <v>F9pPSHdgzwj</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>15-49 years, Male</v>
+        <v>15-19 years, Male</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>lIqSozdCr27</v>
+        <v>sx3u16x80nV</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>2-4 years, Female</v>
+        <v>15-19 years, Unknown Sex</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>H9SWzT8B10p</v>
+        <v>CTWSo1P4qyZ</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>2-4 years, Male</v>
+        <v>20-29 years, Female</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>gMDoZ8IxLFd</v>
+        <v>SIxMfxXNBVo</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>25-34 years, Female</v>
+        <v>20-29 years, Male</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>NZ10jDzwugk</v>
+        <v>bB5hQrGwaD1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>25-34 years, Male</v>
+        <v>20-29 years, Unknown Sex</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AXgnJb5b1Je</v>
+        <v>EjYC7RAtkkQ</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>35-44 years, Female</v>
+        <v>30-39 years, Female</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>FWxLSWmBfd0</v>
+        <v>GiRwR3FD86i</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>35-44 years, Male</v>
+        <v>30-39 years, Male</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>RQChXxsEGmX</v>
+        <v>S17lTK4VVeE</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>45-54 years, Female</v>
+        <v>30-39 years, Unknown Sex</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>VvdznDS1Jcv</v>
+        <v>bAO3xBqTyUk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>45-54 years, Male</v>
+        <v>40-49 years, Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>s8mcd0VkZjn</v>
+        <v>JepUukzD91g</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>5-14 years, Female</v>
+        <v>40-49 years, Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>aIDylQ6ka3n</v>
+        <v>MysvJzZ0ADY</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>5-14 years, Male</v>
+        <v>40-49 years, Unknown Sex</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>bMkvQ4PSTz3</v>
+        <v>ejldVLyrIy7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>50-64 years, Female</v>
+        <v>5-9 years, Female</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>E03CigZ4AM9</v>
+        <v>g5XAclU6mWm</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>50-64 years, Male</v>
+        <v>5-9 years, Male</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Tjy4Mc08yCX</v>
+        <v>bm2siOxEk6w</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>55-64 years, Female</v>
+        <v>5-9 years, Unknown Sex</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>kz9PKqMwjE9</v>
+        <v>S7DctIRHOH4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>55-64 years, Male</v>
+        <v>50-59 years, Female</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>ZTM6ooK5E4V</v>
+        <v>cfJ88kcKfs2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>65-74 years, Female</v>
+        <v>50-59 years, Male</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>L9lGoMl4PWJ</v>
+        <v>Hqno1sfL72D</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>65-74 years, Male</v>
+        <v>50-59 years, Unknown Sex</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>KLFLwpmZLYl</v>
+        <v>nux1VokaZmF</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>65-79 years, Female</v>
+        <v>60-64 years, Female</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>IdLfgkfPvX6</v>
+        <v>ABYB6U68hMU</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>65-79 years, Male</v>
+        <v>60-64 years, Male</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>JtGMAcD0Btm</v>
+        <v>vsG6W671YoN</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>75-84 years, Female</v>
+        <v>60-64 years, Unknown Sex</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>lMo9HzUDdeM</v>
+        <v>YUMOQHnN8pn</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>75-84 years, Male</v>
+        <v>65-69 years, Female</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>F9mySvLgUiB</v>
+        <v>SZ9ccMeGlS6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years, Male</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>FFMPsVh7sxb</v>
+        <v>H0mzaMCOq2e</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>Community transmission</v>
+        <v>65-69 years, Unknown Sex</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>p2ahkO4fbJ9</v>
+        <v>llEP85jmlnN</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>default</v>
+        <v>70-74 years, Female</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>HllvX50cXC0</v>
+        <v>D0g8d1tsNnv</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>ECMO</v>
+        <v>70-74 years, Male</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>cEjvma5H9Il</v>
+        <v>oEsLwo2ah7U</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>Imported</v>
+        <v>70-74 years, Unknown Sex</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>S32sBnGUfwN</v>
+        <v>JC2mJwkcXQ2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>75-79 years, Female</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>tTh6wRIEtFa</v>
+        <v>Lic97hqxsNP</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>Mechanical ventilation</v>
+        <v>75-79 years, Male</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>hJjSk6eIuDt</v>
+        <v>PgmLRiqPKgd</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>75-79 years, Unknown Sex</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>lWjjUr72APP</v>
+        <v>byqkmEDJ42u</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>≥ 85 years, Female</v>
+        <v>80+ years, Female</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>cO1vAjqfkUz</v>
+        <v>RzvnXjQu1cm</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>≥ 85 years, Male</v>
+        <v>80+ years, Male</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>vJ6enc1w0lu</v>
+        <v>zjOFUnSP4cf</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>80+ years, Unknown Sex</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>P6caJBLkaq9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>default</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>2020-03-26</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>HllvX50cXC0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>Female, 0-14 years</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>GHDbaPccoPh</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="str">
+        <v>Male, 0-14 years</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <v>KMTXoNkoiAc</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="str">
+        <v>Unknown age, Female</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <v>w1W0eGecUME</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="str">
+        <v>Unknown age, Male</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <v>BAJrVjxh8K9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="str">
+        <v>Unknown age, Unknown Sex</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <v>meAnvpEpz8M</v>
       </c>
     </row>
   </sheetData>
@@ -952,12 +1034,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -975,46 +1057,24 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>GaGDeErYt4e</v>
+        <v>nd6HGxbW3D5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>CMrvZp5rmoC</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>kJ82l0tJUoe</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>VSS1t1HOSWD</v>
+        <v>XxEFGdwxOJ0</v>
       </c>
     </row>
   </sheetData>
@@ -1023,13 +1083,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1053,10 +1113,10 @@
         <v>0-4 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>0-4 years</v>
+        <v>0-4 y</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yuathFHLjNe</v>
@@ -1064,254 +1124,212 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>15-24 y</v>
+        <v>10-14 y</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>L7gAblMOZKs</v>
+        <v>RoYZKp6iDnH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>25-34 y</v>
+        <v>15-19 y</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>cRskhJQLr4J</v>
+        <v>qiaJA9sMzj2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>35-44 y</v>
+        <v>20-29 y</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>KkZHYvn7Zor</v>
+        <v>p84eezwJhMd</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>45-54 y</v>
+        <v>30-39 y</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>y5yT8JF4uCA</v>
+        <v>u87kL0SUYZa</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>5-14 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>5-14 y</v>
+        <v>40-49 y</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>V9t81g7Wspa</v>
+        <v>nuU9qXctcQE</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 y</v>
+        <v>5-9 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>QllZ8PveFCQ</v>
+        <v>Mcv3dvoK2iM</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74  y</v>
+        <v>50-59 y</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>Y4rNex59t8s</v>
+        <v>IpuKFEXhtUJ</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84  y</v>
+        <v>60-64 y</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>SFZ9S9XHquk</v>
+        <v>JrQqLgsGgFr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>ICU</v>
+        <v>65-69 y</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>XDghoAFhOHg</v>
+        <v>Bap549vCg8U</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 y</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>SKB3wBAOrC2</v>
+        <v>t1JMgMVyoac</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 y</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>QkutHMU0t2V</v>
+        <v>FplLHwIitbU</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ y</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>bqoVhX2RfG4</v>
+        <v>v1e6orGTL3f</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>L8hy5JsqneC</v>
+        <v>bqoVhX2RfG4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>C7gopCwNhoa</v>
+        <v>EVYKU2fIc6G</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Male</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Male</v>
+        <v>Unk Sex</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>EVYKU2fIc6G</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>MV</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>QLONA1SnwU5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <v>QRRRfUrxJs0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>≥ 85 y</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>GL19QsdIgIu</v>
+        <v>SZJNeRyrh22</v>
       </c>
     </row>
   </sheetData>
@@ -1320,13 +1338,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1339,7 +1357,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>0-4 years</v>
@@ -1347,146 +1365,130 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>5-14 years</v>
+        <v>5-9 years</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>40-49 years</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>≥ 85 years</v>
+        <v>65-69 years</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Female</v>
+        <v>70-74 years</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Male</v>
+        <v>75-79 years</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Imported</v>
+        <v>80+ years</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>Male</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>ECMO</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -1500,7 +1502,321 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Options</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Transmission Classification</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>No cases; Sporadic; Clusters; Community</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Option set UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>NzPq5MlxCmh</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>Clusters</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>CLUSTERS</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>zUdhwKZdpT8</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Community</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>COMMUNITY</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>mF5r1p7sKcq</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>No cases</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>NO_CASES</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>AXl3Z9rLjLi</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>Sporadic</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>SPORADIC</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Instruction</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Left side</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Operator</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Right side</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>New Cases hospitalised should be less than or equal to All new cases reported</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>New Cases hospitalised</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>All New Cases</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>bO8rXNzj0iR</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Test with PCR should be less than or equal to tested</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>Tested with PCR</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>Tested</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <v>gZwUbrTOa0g</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>WY7h5pKok2I</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Validation Rule Group</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Validation Rule</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1522,36 +1838,99 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19</v>
+        <v>COVID19</v>
       </c>
       <c r="B2" s="4" t="str">
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Property</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Name:</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>Custom form:</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Sections:</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>UID:</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>uKtOZwDnIpM</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="153.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
@@ -1591,16 +1970,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>zUcGi0Y384Y</v>
+        <v>ZTklbd8JtLn</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - Active cases</v>
+        <v>COVID19 - Active cases</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Active cases</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v/>
+        <v>CV19_ACTIVE_CASES</v>
       </c>
       <c r="E2" s="4" t="str">
         <v/>
@@ -1615,94 +1994,94 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>kJoSHTinHGa</v>
+        <v>LeNVLm6SL1x</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - All cases</v>
+        <v>COVID19 - Case fatality rate (%)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>All cases</v>
+        <v>Case Fatality rate (%)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE</v>
       </c>
       <c r="E3" s="5" t="str">
         <v/>
       </c>
       <c r="F3" s="5" t="str">
-        <v>All cases</v>
+        <v>Death (Confirmed + Probable)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J3" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>dXAhOKiim1x</v>
+        <v>NP88sGFKpCQ</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Case Fatality rate (%)</v>
+        <v>COVID19 - Case fatality rate among HW (%)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Case Fatality rate (%)</v>
+        <v>Case fatality rate HW (%)</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE_HW</v>
       </c>
       <c r="E4" s="4" t="str">
         <v/>
       </c>
       <c r="F4" s="4" t="str">
-        <v>Deaths Reported</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="H4" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J4" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>fK1b7O6CuBV</v>
+        <v>VJHMO9gHkV5</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Cases treated by mechanical ventilation, ECMO or ICU</v>
+        <v>COVID19 - Closed cases</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Cases treated by type</v>
+        <v>Closed cases</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v/>
+        <v>CV19_CLOSED_CASES</v>
       </c>
       <c r="E5" s="5" t="str">
         <v/>
       </c>
       <c r="F5" s="5" t="str">
-        <v>Number of suspected cases that received mechanical ventilation, ECMO or admitted into intensive care unit</v>
+        <v>Closed cases</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>1</v>
@@ -1711,30 +2090,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J5" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>S3Ty19GEaqn</v>
+        <v>TmKNBHtBx6D</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Closed cases</v>
+        <v>COVID19 - New Confirmed cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Closed cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="E6" s="4" t="str">
         <v/>
       </c>
       <c r="F6" s="4" t="str">
-        <v>Active Cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>1</v>
@@ -1743,30 +2122,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J6" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>ocBlGrHZy6Q</v>
+        <v>yzyWxXoSCny</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Confirmed cases</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="E7" s="5" t="str">
         <v/>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Suspected cases that were confirmed through laboratory testing (multiple lab tests may be conducted; this indicator assumes that the last test result).</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>1</v>
@@ -1775,30 +2154,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J7" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zozhRzInMZm</v>
+        <v>U89bOzPbFyA</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by Transmission Classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="E8" s="4" t="str">
         <v/>
       </c>
       <c r="F8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>1</v>
@@ -1807,30 +2186,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J8" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>r2VxAVW1IEy</v>
+        <v>DnleIypnqxJ</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - Deaths</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Deaths</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="E9" s="5" t="str">
         <v/>
       </c>
       <c r="F9" s="5" t="str">
-        <v>COVID-19 related deaths (deaths recorded among all suspected cases)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -1839,158 +2218,158 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J9" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>BmW2IAaxIBe</v>
+        <v>C6A59SObXV6</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - Hospitalised Cases</v>
+        <v>COVID19 - Positivity rate (%)</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Hospitalised Cases</v>
+        <v>Positivity rate (%)</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v/>
+        <v>CV19_POSITIVITY_RATE</v>
       </c>
       <c r="E10" s="4" t="str">
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <v>Number of suspected or confirmed or probable cases that were admitted into hospital</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>1</v>
+        <v>Tested</v>
       </c>
       <c r="H10" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J10" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>jHzx1zXeHzV</v>
+        <v>x6IelBioEX1</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Proportion of males among confirmed cases (%)</v>
+        <v>COVID19 - Proportion of HW amongst reported cases (%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Proportion of males among confirmed cases (%)</v>
+        <v>HW among confirmed cases (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v/>
+        <v>CV19_%_HW_AMONGST_REPORTED_CASES</v>
       </c>
       <c r="E11" s="5" t="str">
         <v/>
       </c>
       <c r="F11" s="5" t="str">
-        <v>Males among confirmed cases</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="H11" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J11" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>UF7s1t1v6KG</v>
+        <v>cJZS7kSFFGl</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - Proportion of males among deaths(%)</v>
+        <v>COVID19 - Proportion of PCR tests (%)</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Proportion of males among deaths (%)</v>
+        <v>Proportion of PCR tests</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v/>
+        <v>CV19_%_PCR_TESTS</v>
       </c>
       <c r="E12" s="4" t="str">
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <v>Males among deaths</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>Deaths</v>
+        <v>Tested</v>
       </c>
       <c r="H12" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J12" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>gYt2GEAdCJK</v>
+        <v>K2JqazsxhvP</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Recovery rate (%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Recovery rate (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v/>
+        <v>CV19_RECOVERY_RATE</v>
       </c>
       <c r="E13" s="5" t="str">
         <v/>
       </c>
       <c r="F13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J13" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>JpRDu51rbg5</v>
+        <v>pxqFjCNLkzD</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v/>
+        <v>CV19_TESTED</v>
       </c>
       <c r="E14" s="4" t="str">
         <v/>
       </c>
       <c r="F14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>1</v>
@@ -1999,30 +2378,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J14" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>vECy4BgZqRF</v>
+        <v>jgyO0rV708H</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (No cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v/>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="E15" s="5" t="str">
         <v/>
       </c>
       <c r="F15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>1</v>
@@ -2031,113 +2410,17 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J15" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>GszrLGBvHhg</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="G16" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>PkGdfHQyWWH</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>COVID-19 - Recovered cases</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>Recovered cases</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>Number of cases that are recovered.</v>
-      </c>
-      <c r="G17" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I17" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J17" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>dsho3rAaUkr</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>COVID-19 - Recovery rate (%)</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>Case Recovery rate</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>Cases Recovered</v>
-      </c>
-      <c r="G18" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
-      </c>
-      <c r="H18" s="4" t="str">
-        <v>Percentage</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J18" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2172,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2018-01-16</v>
+        <v>2020-09-09</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>kHy61PbChXr</v>
@@ -2196,14 +2479,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2221,29 +2504,29 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>04. COVID-19 Surveillance (Aggregate)</v>
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="93.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -2271,356 +2554,236 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>ud3dbLWVafm</v>
+        <v>jTGq07MlmMp</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>ZcYLgBQrhgu</v>
+        <v>btrkVNdRwnO</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>n2mZrxngMFR</v>
+        <v>oaBx9hR7FFR</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>nIVBxZaZ8Gd</v>
+        <v>jmn7HoMmBHC</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>FjfJIiULctQ</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>lIAZDq6H4dF</v>
+        <v>JNHOYQEIN3V</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>o9HS22p81W0</v>
+        <v>P7syfXG9dNm</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>E6w4iwPkaRM</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>YzYCsOsZDz2</v>
+        <v>IeZQZcgmAfV</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>dFmHVADG2t5</v>
+        <v>KWM5EsM8hYR</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>WcRHBfw09Iq</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>cSmHf59IIs5</v>
+        <v>qTkvVnIP5Ri</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E94X1H21okK</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>kz9Z0mKZQbN</v>
+        <v>KMsy5gLLUWr</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>neIuzgRUO0N</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>hoZsDsseA6B</v>
+        <v>JZ4Jt9JxsVh</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>p6zlpJrZzJV</v>
+        <v>pQ6jw6r59Op</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>kQCzFsC1eEU</v>
+        <v>YocjDGUCP18</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>cTcbZ8ht1zi</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>r83aoS5wveR</v>
+        <v>dbn6GloPaRP</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>GjZAEBGomjW</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>KYC90zR9e6n</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>VvJv2JhRgLE</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>h0FivHWebim</v>
-      </c>
-      <c r="E15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F15" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>HrI5yNYmham</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v>GvYhMDZrNH9</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v>hOLM46Ckolu</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>WSZu4jpViok</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>NMmB1l6X07Y</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="93.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2642,281 +2805,142 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>KYC90zR9e6n</v>
+        <v>pQ6jw6r59Op</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>HrI5yNYmham</v>
+        <v>neIuzgRUO0N</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>E94X1H21okK</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E6w4iwPkaRM</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="B7" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
+        <v>WcRHBfw09Iq</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>WSZu4jpViok</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
+        <v>oaBx9hR7FFR</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="B10" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>FjfJIiULctQ</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>n2mZrxngMFR</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>ud3dbLWVafm</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>cTcbZ8ht1zi</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Custom form</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Sections</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v>No</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>kIfMNugiTgd</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>No</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>Vs7Bd0pHjS9</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2938,37 +2962,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>p6zlpJrZzJV</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>jTGq07MlmMp</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2997,23 +3007,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3042,44 +3052,44 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>hZvJeK3Imky</v>
+        <v>BigUFwCduUF</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>V7qvIqRNyhQ</v>
+        <v>y9n0wxeewlR</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3100,7 +3110,7 @@
         <v>COVID19 access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-04-24</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>DoYehxUvmwT</v>
@@ -3111,28 +3121,17 @@
         <v>COVID19 admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-21</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>w4iJeNKy9br</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID19 data capture</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>k8Fk0kuhOeK</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3157,13 +3156,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>who</v>
+        <v>covid19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2018-07-13</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>vUeLeQMSwhN</v>
+        <v>F0YhCM0Pi73</v>
       </c>
     </row>
   </sheetData>
@@ -3172,99 +3171,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Section name</v>
+        <v>Last updated</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>BF8373CGyyT</v>
+        <v>i9rpQqB3Hfh</v>
       </c>
     </row>
   </sheetData>
@@ -3273,254 +3209,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="77.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Data Set Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Data Set Section</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Section UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>Data Element</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>Data Element UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
-      </c>
-      <c r="E7" s="5" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>njg6PAh5gw6</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
-      </c>
-      <c r="E12" s="4" t="str">
-        <v>e1xTRwfWega</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>h34jPNnKkJK</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>RC7RG6mexD2</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
   </sheetData>
@@ -3529,16 +3320,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3568,13 +3359,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases tested</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID_19_CASES_TESTED</v>
+        <v>CV19_NEW_CONF_PROB_HW_CASES</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
@@ -3583,136 +3374,136 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>SU1j9CmCuW9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Confirmed cases by transmission classification</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID_19_CONFIRMED_CASES_BY_TC</v>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>bmbNyNoJcXP</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>New cases hospitalised</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID_19_NEW_CASES_HOSPITALISED</v>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>default</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>rBw83gVQLHK</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - New cases treated</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>New cases treated</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID_19_NEW_CASES_TREATED</v>
+        <v>CV19_NEW_CONF_PROB_HW_DEATHS</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>DI9JgEJ3t8v</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>New confirmed cases (sex/age)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID_19_NEW_CONFIRMED_CASES</v>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>fJ7Qi1zcdAR</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>New deaths (sex/age)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID_19_NEW_DEATHS</v>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>cW0odY9vhrd</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New Suspected cases (sex/age)</v>
+        <v>New Probable Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID_19_NEW_SUSPECTED_CASES</v>
+        <v>CV19_NEW_PROB_CASES</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -3721,21 +3512,21 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>VnkErE22ELJ</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Recovered cases (sex/age)</v>
+        <v>New Probable Deaths</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID_19_RECOVERED_CASES</v>
+        <v>CV19_NEW_PROB_DEATHS</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -3744,44 +3535,44 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G9" s="5" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>N59eghaBpM7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Suspected cases by transmission classification</v>
+        <v>Tested</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID_19_SUSPECTED_CASES_BY_TC</v>
+        <v>CV19_TESTED</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
       </c>
       <c r="E10" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>E1pXvzyZzKB</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>COVID_19_TP_CLUSTER_CASES</v>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="D11" s="5" t="str">
         <v/>
@@ -3790,21 +3581,21 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>e1xTRwfWega</v>
+        <v>pZtyMNtYPLM</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern (Community  cases)</v>
+        <v>Transmission Classification</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID_19_TP_COMMUNITY_CASES</v>
+        <v>CV19_TRANS_CLASS</v>
       </c>
       <c r="D12" s="4" t="str">
         <v/>
@@ -3813,56 +3604,10 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>RC7RG6mexD2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID_19_TP_NO_CASES</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>default</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <v>njg6PAh5gw6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>COVID_19_TP_SPORADIC_CASES</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>default</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G14" s="4" t="str">
-        <v>h34jPNnKkJK</v>
+        <v>sWCFbUawFDa</v>
       </c>
     </row>
   </sheetData>
@@ -3871,13 +3616,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3893,7 +3638,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
     <row r="3">
@@ -3901,7 +3646,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
@@ -3909,7 +3654,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
@@ -3917,7 +3662,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="6">
@@ -3925,7 +3670,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="7">
@@ -3933,7 +3678,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="8">
@@ -3941,7 +3686,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="9">
@@ -3949,7 +3694,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="10">
@@ -3957,7 +3702,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="11">
@@ -3965,7 +3710,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="12">
@@ -3973,23 +3718,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
   </sheetData>
@@ -3998,15 +3727,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4028,13 +3757,13 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>o3OiZXHwBzY</v>
+        <v>UPxdJOxz2I7</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Age (COVID-19); Sex</v>
+        <v>Age (COVID19); Sex (with unknown)</v>
       </c>
     </row>
     <row r="3">
@@ -4042,41 +3771,13 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2017-05-28</v>
+        <v>2020-05-11</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bjDvmb4bfuf</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>default</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>FGDN1aBqJnt</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>sRwqVdFcBat</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
       </c>
     </row>
   </sheetData>
@@ -4085,15 +3786,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="126.7109375" customWidth="1"/>
+    <col min="4" max="4" width="176.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4112,16 +3813,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age (COVID-19)</v>
+        <v>Age (COVID19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>prZlmHqhxLO</v>
+        <v>RrZWSJ6CsLs</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>0-4 years; 5-14 years; 15-24 years; 25-34 years; 35-44 years; 45-54 years; 55-64 years; 65-74 years; 75-84 years; ≥ 85 years</v>
+        <v>0-4 years; 5-9 years; 10-14 years; 15-19 years; 20-29 years; 30-39 years; 40-49 years; 50-59 years; 60-64 years; 65-69 years; 70-74 years; 75-79 years; 80+ years; Unknown age</v>
       </c>
     </row>
     <row r="3">
@@ -4129,7 +3830,7 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-13</v>
+        <v>2020-10-01</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>GLevLNI9wkl</v>
@@ -4140,44 +3841,16 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Sex</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-22</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>FRwO58KwwJt</v>
+        <v>b7peexUktxt</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Male; Female</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>v1atVR1HnCr</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Imported; Known Cluster; Community transmission; Unknown Classification</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>PWWzA79GcCG</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>Mechanical ventilation; ECMO; Admitted in intensive care unit (ICU)</v>
+        <v>Male; Female; Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -4186,12 +3859,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4209,13 +3882,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years</v>
+        <v>0-14 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2019-07-03</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>uueCp2RIGCJ</v>
+        <v>IoqDBYr0rH5</v>
       </c>
     </row>
     <row r="3">
@@ -4223,7 +3896,7 @@
         <v>0-4 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>UPvKbcqTEY3</v>
@@ -4231,255 +3904,189 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>ls9vGYWbvwG</v>
+        <v>ftXCKvbuGgj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>15-49 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jqg45gLQRYI</v>
+        <v>dENFBee17Oi</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>2-4 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>jxOEQ4Ss4bM</v>
+        <v>GERCWxK3mvz</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>25-34 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>O6UJSfL4psp</v>
+        <v>bY3NyagrzeD</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>35-44 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>utyLRFta4ie</v>
+        <v>tTmsWzvoEUv</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>45-54 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>nkQw9lhkbGV</v>
+        <v>J205eXYNH7q</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>5-14 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>pa0cY66MrG6</v>
+        <v>BOCPEdURsYX</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>50-64 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Yl34dHOPpZ0</v>
+        <v>TEBfAmuOSJk</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>55-64 years</v>
+        <v>65-69 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Lo1gxiS8zap</v>
+        <v>gHA96noC0iO</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>65-74 years</v>
+        <v>70-74 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AlUYlzoMVvN</v>
+        <v>Po7T5dd3tQs</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>65-79 years</v>
+        <v>75-79 years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>ZPzdstvH08a</v>
+        <v>xWXUBYNycnE</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>75-84 years</v>
+        <v>80+ years</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>R4m7KraS4aZ</v>
+        <v>c2hLbh0drQI</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>default</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2018-05-30</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>zUAhtH6iiyz</v>
+        <v>xYerKDKCefk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>hH4LYNplIeA</v>
+        <v>FFA9e1yIXCT</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>default</v>
+        <v>Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2018-05-30</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>xYerKDKCefk</v>
+        <v>MP15bHaQh2x</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>ECMO</v>
+        <v>Unknown age</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>mg1cBsgdqHC</v>
+        <v>WNPpyVkVaL3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>Female</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>FFA9e1yIXCT</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="str">
-        <v>Imported</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>y8TxHRrY1eN</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="str">
-        <v>Known Cluster</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C22" s="4" t="str">
-        <v>LIRv9sIHNOD</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="str">
-        <v>Male</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <v>MP15bHaQh2x</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <v>qoxRSWYj9cB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <v>YfLFBoAcjE2</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <v>F3RlEj6nnR3</v>
+        <v>kuP5EmQRFke</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add package for D2.31
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -16,17 +16,22 @@
     <sheet name="categoryOptionGroupSets" sheetId="11" r:id="rId11"/>
     <sheet name="categoryOptionGroups" sheetId="12" r:id="rId12"/>
     <sheet name="categoryOptionGroupsBySet" sheetId="13" r:id="rId13"/>
-    <sheet name="indicatorGroups" sheetId="14" r:id="rId14"/>
-    <sheet name="indicators" sheetId="15" r:id="rId15"/>
-    <sheet name="indicatorTypes" sheetId="16" r:id="rId16"/>
-    <sheet name="dashboards" sheetId="17" r:id="rId17"/>
-    <sheet name="dashboardItems" sheetId="18" r:id="rId18"/>
-    <sheet name="charts" sheetId="19" r:id="rId19"/>
-    <sheet name="reportTables" sheetId="20" r:id="rId20"/>
-    <sheet name="maps" sheetId="21" r:id="rId21"/>
-    <sheet name="mapViews" sheetId="22" r:id="rId22"/>
-    <sheet name="userGroups" sheetId="23" r:id="rId23"/>
-    <sheet name="users" sheetId="24" r:id="rId24"/>
+    <sheet name="optionSets" sheetId="14" r:id="rId14"/>
+    <sheet name="options" sheetId="15" r:id="rId15"/>
+    <sheet name="validationRules" sheetId="16" r:id="rId16"/>
+    <sheet name="validationRuleGroups" sheetId="17" r:id="rId17"/>
+    <sheet name="validationRules by group" sheetId="18" r:id="rId18"/>
+    <sheet name="indicatorGroups" sheetId="19" r:id="rId19"/>
+    <sheet name="indicators" sheetId="20" r:id="rId20"/>
+    <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
+    <sheet name="dashboards" sheetId="22" r:id="rId22"/>
+    <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
+    <sheet name="maps" sheetId="26" r:id="rId26"/>
+    <sheet name="mapViews" sheetId="27" r:id="rId27"/>
+    <sheet name="userGroups" sheetId="28" r:id="rId28"/>
+    <sheet name="users" sheetId="29" r:id="rId29"/>
   </sheets>
 </workbook>
 </file>
@@ -442,7 +447,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -466,7 +471,7 @@
         <v>Type</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>AGG</v>
+        <v>COMPLETE</v>
       </c>
     </row>
     <row r="4">
@@ -474,7 +479,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COMPLETE</v>
+        <v>V2.0</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +487,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>V1.0.1</v>
+        <v>DHIS2.31</v>
       </c>
     </row>
     <row r="6">
@@ -490,7 +495,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>DHIS2.31</v>
+        <v>2020-10-12T14:22</v>
       </c>
     </row>
     <row r="7">
@@ -498,7 +503,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID19_AGG_COMPLETE_V1.0.1_DHIS2.31_2020-03-27T08:26</v>
+        <v>COVID19_COMPLETE_V2.0_DHIS2.31_2020-10-12T14:22</v>
       </c>
     </row>
   </sheetData>
@@ -507,12 +512,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -530,420 +535,497 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years, Female</v>
+        <v>0-4 years, Female</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>h72VZMAIXNp</v>
+        <v>X7SGUlfmJa5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>0-1 years, Male</v>
+        <v>0-4 years, Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>NZkmbtZAFtN</v>
+        <v>d1XzGx028Z8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>0-4 years, Female</v>
+        <v>0-4 years, Unknown Sex</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>JzrkRqzvWhH</v>
+        <v>Ter1Z3EGkQM</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>0-4 years, Male</v>
+        <v>10-14 years, Female</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jQqLIn3xasU</v>
+        <v>vvpjmqp0psR</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>15-24 years, Female</v>
+        <v>10-14 years, Male</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>gPWH4piZwC0</v>
+        <v>SV1RvPdmAkj</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>15-24 years, Male</v>
+        <v>10-14 years, Unknown Sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>uhLnCuMwCGm</v>
+        <v>XUXU9zyHXN9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>15-49 years, Female</v>
+        <v>15-19 years, Female</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>sFJsKLHLBFj</v>
+        <v>F9pPSHdgzwj</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>15-49 years, Male</v>
+        <v>15-19 years, Male</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>lIqSozdCr27</v>
+        <v>sx3u16x80nV</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>2-4 years, Female</v>
+        <v>15-19 years, Unknown Sex</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>H9SWzT8B10p</v>
+        <v>CTWSo1P4qyZ</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>2-4 years, Male</v>
+        <v>20-29 years, Female</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>gMDoZ8IxLFd</v>
+        <v>SIxMfxXNBVo</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>25-34 years, Female</v>
+        <v>20-29 years, Male</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>NZ10jDzwugk</v>
+        <v>bB5hQrGwaD1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>25-34 years, Male</v>
+        <v>20-29 years, Unknown Sex</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AXgnJb5b1Je</v>
+        <v>EjYC7RAtkkQ</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>35-44 years, Female</v>
+        <v>30-39 years, Female</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>FWxLSWmBfd0</v>
+        <v>GiRwR3FD86i</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>35-44 years, Male</v>
+        <v>30-39 years, Male</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>RQChXxsEGmX</v>
+        <v>S17lTK4VVeE</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>45-54 years, Female</v>
+        <v>30-39 years, Unknown Sex</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>VvdznDS1Jcv</v>
+        <v>bAO3xBqTyUk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>45-54 years, Male</v>
+        <v>40-49 years, Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>s8mcd0VkZjn</v>
+        <v>JepUukzD91g</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>5-14 years, Female</v>
+        <v>40-49 years, Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>aIDylQ6ka3n</v>
+        <v>MysvJzZ0ADY</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>5-14 years, Male</v>
+        <v>40-49 years, Unknown Sex</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>bMkvQ4PSTz3</v>
+        <v>ejldVLyrIy7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>50-64 years, Female</v>
+        <v>5-9 years, Female</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>E03CigZ4AM9</v>
+        <v>g5XAclU6mWm</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>50-64 years, Male</v>
+        <v>5-9 years, Male</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Tjy4Mc08yCX</v>
+        <v>bm2siOxEk6w</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>55-64 years, Female</v>
+        <v>5-9 years, Unknown Sex</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>kz9PKqMwjE9</v>
+        <v>S7DctIRHOH4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>55-64 years, Male</v>
+        <v>50-59 years, Female</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>ZTM6ooK5E4V</v>
+        <v>cfJ88kcKfs2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>65-74 years, Female</v>
+        <v>50-59 years, Male</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>L9lGoMl4PWJ</v>
+        <v>Hqno1sfL72D</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>65-74 years, Male</v>
+        <v>50-59 years, Unknown Sex</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>KLFLwpmZLYl</v>
+        <v>nux1VokaZmF</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>65-79 years, Female</v>
+        <v>60-64 years, Female</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>IdLfgkfPvX6</v>
+        <v>ABYB6U68hMU</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>65-79 years, Male</v>
+        <v>60-64 years, Male</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>JtGMAcD0Btm</v>
+        <v>vsG6W671YoN</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>75-84 years, Female</v>
+        <v>60-64 years, Unknown Sex</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>lMo9HzUDdeM</v>
+        <v>YUMOQHnN8pn</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>75-84 years, Male</v>
+        <v>65-69 years, Female</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>F9mySvLgUiB</v>
+        <v>SZ9ccMeGlS6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years, Male</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>FFMPsVh7sxb</v>
+        <v>H0mzaMCOq2e</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>Community transmission</v>
+        <v>65-69 years, Unknown Sex</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>p2ahkO4fbJ9</v>
+        <v>llEP85jmlnN</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>default</v>
+        <v>70-74 years, Female</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>HllvX50cXC0</v>
+        <v>D0g8d1tsNnv</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>ECMO</v>
+        <v>70-74 years, Male</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>cEjvma5H9Il</v>
+        <v>oEsLwo2ah7U</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>Imported</v>
+        <v>70-74 years, Unknown Sex</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>S32sBnGUfwN</v>
+        <v>JC2mJwkcXQ2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>75-79 years, Female</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>tTh6wRIEtFa</v>
+        <v>Lic97hqxsNP</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>Mechanical ventilation</v>
+        <v>75-79 years, Male</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>hJjSk6eIuDt</v>
+        <v>PgmLRiqPKgd</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>75-79 years, Unknown Sex</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>lWjjUr72APP</v>
+        <v>byqkmEDJ42u</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>≥ 85 years, Female</v>
+        <v>80+ years, Female</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>cO1vAjqfkUz</v>
+        <v>RzvnXjQu1cm</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>≥ 85 years, Male</v>
+        <v>80+ years, Male</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>vJ6enc1w0lu</v>
+        <v>zjOFUnSP4cf</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>80+ years, Unknown Sex</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>P6caJBLkaq9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>default</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>2020-03-26</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>HllvX50cXC0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>Female, 0-14 years</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>GHDbaPccoPh</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="str">
+        <v>Male, 0-14 years</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <v>KMTXoNkoiAc</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="str">
+        <v>Unknown age, Female</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <v>w1W0eGecUME</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="str">
+        <v>Unknown age, Male</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <v>BAJrVjxh8K9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="str">
+        <v>Unknown age, Unknown Sex</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <v>meAnvpEpz8M</v>
       </c>
     </row>
   </sheetData>
@@ -952,12 +1034,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -975,46 +1057,24 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>GaGDeErYt4e</v>
+        <v>nd6HGxbW3D5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>CMrvZp5rmoC</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>kJ82l0tJUoe</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>VSS1t1HOSWD</v>
+        <v>XxEFGdwxOJ0</v>
       </c>
     </row>
   </sheetData>
@@ -1023,13 +1083,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1053,10 +1113,10 @@
         <v>0-4 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>0-4 years</v>
+        <v>0-4 y</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yuathFHLjNe</v>
@@ -1064,254 +1124,212 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>15-24 y</v>
+        <v>10-14 y</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>L7gAblMOZKs</v>
+        <v>RoYZKp6iDnH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>25-34 y</v>
+        <v>15-19 y</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>cRskhJQLr4J</v>
+        <v>qiaJA9sMzj2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>35-44 y</v>
+        <v>20-29 y</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>KkZHYvn7Zor</v>
+        <v>p84eezwJhMd</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>45-54 y</v>
+        <v>30-39 y</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>y5yT8JF4uCA</v>
+        <v>u87kL0SUYZa</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>5-14 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>5-14 y</v>
+        <v>40-49 y</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>V9t81g7Wspa</v>
+        <v>nuU9qXctcQE</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 y</v>
+        <v>5-9 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>QllZ8PveFCQ</v>
+        <v>Mcv3dvoK2iM</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74  y</v>
+        <v>50-59 y</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>Y4rNex59t8s</v>
+        <v>IpuKFEXhtUJ</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84  y</v>
+        <v>60-64 y</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>SFZ9S9XHquk</v>
+        <v>JrQqLgsGgFr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>ICU</v>
+        <v>65-69 y</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>XDghoAFhOHg</v>
+        <v>Bap549vCg8U</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 y</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>SKB3wBAOrC2</v>
+        <v>t1JMgMVyoac</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 y</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>QkutHMU0t2V</v>
+        <v>FplLHwIitbU</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ y</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>bqoVhX2RfG4</v>
+        <v>v1e6orGTL3f</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>L8hy5JsqneC</v>
+        <v>bqoVhX2RfG4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>C7gopCwNhoa</v>
+        <v>EVYKU2fIc6G</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Male</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Male</v>
+        <v>Unk Sex</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>EVYKU2fIc6G</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>MV</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>QLONA1SnwU5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <v>QRRRfUrxJs0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>≥ 85 y</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>GL19QsdIgIu</v>
+        <v>SZJNeRyrh22</v>
       </c>
     </row>
   </sheetData>
@@ -1320,13 +1338,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1339,7 +1357,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>0-4 years</v>
@@ -1347,146 +1365,130 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>5-14 years</v>
+        <v>5-9 years</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>40-49 years</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>≥ 85 years</v>
+        <v>65-69 years</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Female</v>
+        <v>70-74 years</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Male</v>
+        <v>75-79 years</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Imported</v>
+        <v>80+ years</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>Male</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>ECMO</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -1500,7 +1502,321 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Options</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Transmission Classification</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>No cases; Sporadic; Clusters; Community</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Option set UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>NzPq5MlxCmh</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>Clusters</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>CLUSTERS</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>zUdhwKZdpT8</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Community</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>COMMUNITY</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>mF5r1p7sKcq</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>No cases</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>NO_CASES</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>AXl3Z9rLjLi</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>Sporadic</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>SPORADIC</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Instruction</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Left side</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Operator</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Right side</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>New Cases hospitalised should be less than or equal to All new cases reported</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>New Cases hospitalised</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>All New Cases</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>bO8rXNzj0iR</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Test with PCR should be less than or equal to tested</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>Tested with PCR</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>Tested</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <v>gZwUbrTOa0g</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>WY7h5pKok2I</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Validation Rule Group</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Validation Rule</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1522,36 +1838,99 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19</v>
+        <v>COVID19</v>
       </c>
       <c r="B2" s="4" t="str">
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Property</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Name:</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>Custom form:</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Sections:</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>UID:</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>uKtOZwDnIpM</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="153.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
@@ -1591,16 +1970,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>zUcGi0Y384Y</v>
+        <v>ZTklbd8JtLn</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - Active cases</v>
+        <v>COVID19 - Active cases</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Active cases</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v/>
+        <v>CV19_ACTIVE_CASES</v>
       </c>
       <c r="E2" s="4" t="str">
         <v/>
@@ -1615,94 +1994,94 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>kJoSHTinHGa</v>
+        <v>LeNVLm6SL1x</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - All cases</v>
+        <v>COVID19 - Case fatality rate (%)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>All cases</v>
+        <v>Case Fatality rate (%)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE</v>
       </c>
       <c r="E3" s="5" t="str">
         <v/>
       </c>
       <c r="F3" s="5" t="str">
-        <v>All cases</v>
+        <v>Death (Confirmed + Probable)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J3" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>dXAhOKiim1x</v>
+        <v>NP88sGFKpCQ</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Case Fatality rate (%)</v>
+        <v>COVID19 - Case fatality rate among HW (%)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Case Fatality rate (%)</v>
+        <v>Case fatality rate HW (%)</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE_HW</v>
       </c>
       <c r="E4" s="4" t="str">
         <v/>
       </c>
       <c r="F4" s="4" t="str">
-        <v>Deaths Reported</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="H4" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J4" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>fK1b7O6CuBV</v>
+        <v>VJHMO9gHkV5</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Cases treated by mechanical ventilation, ECMO or ICU</v>
+        <v>COVID19 - Closed cases</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Cases treated by type</v>
+        <v>Closed cases</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v/>
+        <v>CV19_CLOSED_CASES</v>
       </c>
       <c r="E5" s="5" t="str">
         <v/>
       </c>
       <c r="F5" s="5" t="str">
-        <v>Number of suspected cases that received mechanical ventilation, ECMO or admitted into intensive care unit</v>
+        <v>Closed cases</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>1</v>
@@ -1711,30 +2090,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J5" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>S3Ty19GEaqn</v>
+        <v>TmKNBHtBx6D</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Closed cases</v>
+        <v>COVID19 - New Confirmed cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Closed cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="E6" s="4" t="str">
         <v/>
       </c>
       <c r="F6" s="4" t="str">
-        <v>Active Cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>1</v>
@@ -1743,30 +2122,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J6" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>ocBlGrHZy6Q</v>
+        <v>yzyWxXoSCny</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Confirmed cases</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="E7" s="5" t="str">
         <v/>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Suspected cases that were confirmed through laboratory testing (multiple lab tests may be conducted; this indicator assumes that the last test result).</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>1</v>
@@ -1775,30 +2154,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J7" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zozhRzInMZm</v>
+        <v>U89bOzPbFyA</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by Transmission Classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="E8" s="4" t="str">
         <v/>
       </c>
       <c r="F8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>1</v>
@@ -1807,30 +2186,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J8" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>r2VxAVW1IEy</v>
+        <v>DnleIypnqxJ</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - Deaths</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Deaths</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="E9" s="5" t="str">
         <v/>
       </c>
       <c r="F9" s="5" t="str">
-        <v>COVID-19 related deaths (deaths recorded among all suspected cases)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -1839,158 +2218,158 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J9" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>BmW2IAaxIBe</v>
+        <v>C6A59SObXV6</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - Hospitalised Cases</v>
+        <v>COVID19 - Positivity rate (%)</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Hospitalised Cases</v>
+        <v>Positivity rate (%)</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v/>
+        <v>CV19_POSITIVITY_RATE</v>
       </c>
       <c r="E10" s="4" t="str">
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <v>Number of suspected or confirmed or probable cases that were admitted into hospital</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>1</v>
+        <v>Tested</v>
       </c>
       <c r="H10" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J10" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>jHzx1zXeHzV</v>
+        <v>x6IelBioEX1</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Proportion of males among confirmed cases (%)</v>
+        <v>COVID19 - Proportion of HW amongst reported cases (%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Proportion of males among confirmed cases (%)</v>
+        <v>HW among confirmed cases (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v/>
+        <v>CV19_%_HW_AMONGST_REPORTED_CASES</v>
       </c>
       <c r="E11" s="5" t="str">
         <v/>
       </c>
       <c r="F11" s="5" t="str">
-        <v>Males among confirmed cases</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="H11" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J11" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>UF7s1t1v6KG</v>
+        <v>cJZS7kSFFGl</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - Proportion of males among deaths(%)</v>
+        <v>COVID19 - Proportion of PCR tests (%)</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Proportion of males among deaths (%)</v>
+        <v>Proportion of PCR tests</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v/>
+        <v>CV19_%_PCR_TESTS</v>
       </c>
       <c r="E12" s="4" t="str">
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <v>Males among deaths</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>Deaths</v>
+        <v>Tested</v>
       </c>
       <c r="H12" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J12" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>gYt2GEAdCJK</v>
+        <v>K2JqazsxhvP</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Recovery rate (%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Recovery rate (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v/>
+        <v>CV19_RECOVERY_RATE</v>
       </c>
       <c r="E13" s="5" t="str">
         <v/>
       </c>
       <c r="F13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J13" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>JpRDu51rbg5</v>
+        <v>pxqFjCNLkzD</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v/>
+        <v>CV19_TESTED</v>
       </c>
       <c r="E14" s="4" t="str">
         <v/>
       </c>
       <c r="F14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>1</v>
@@ -1999,30 +2378,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J14" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>vECy4BgZqRF</v>
+        <v>jgyO0rV708H</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (No cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v/>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="E15" s="5" t="str">
         <v/>
       </c>
       <c r="F15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>1</v>
@@ -2031,113 +2410,17 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J15" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>GszrLGBvHhg</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="G16" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>PkGdfHQyWWH</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>COVID-19 - Recovered cases</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>Recovered cases</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>Number of cases that are recovered.</v>
-      </c>
-      <c r="G17" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I17" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J17" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>dsho3rAaUkr</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>COVID-19 - Recovery rate (%)</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>Case Recovery rate</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>Cases Recovered</v>
-      </c>
-      <c r="G18" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
-      </c>
-      <c r="H18" s="4" t="str">
-        <v>Percentage</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J18" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2172,7 +2455,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2018-01-16</v>
+        <v>2020-09-09</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>kHy61PbChXr</v>
@@ -2196,14 +2479,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2221,29 +2504,29 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>04. COVID-19 Surveillance (Aggregate)</v>
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="93.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -2271,356 +2554,236 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>ud3dbLWVafm</v>
+        <v>jTGq07MlmMp</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>ZcYLgBQrhgu</v>
+        <v>btrkVNdRwnO</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>n2mZrxngMFR</v>
+        <v>oaBx9hR7FFR</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>nIVBxZaZ8Gd</v>
+        <v>jmn7HoMmBHC</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>FjfJIiULctQ</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>lIAZDq6H4dF</v>
+        <v>JNHOYQEIN3V</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>o9HS22p81W0</v>
+        <v>P7syfXG9dNm</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>E6w4iwPkaRM</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>YzYCsOsZDz2</v>
+        <v>IeZQZcgmAfV</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>dFmHVADG2t5</v>
+        <v>KWM5EsM8hYR</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>WcRHBfw09Iq</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>cSmHf59IIs5</v>
+        <v>qTkvVnIP5Ri</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E94X1H21okK</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>kz9Z0mKZQbN</v>
+        <v>KMsy5gLLUWr</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>neIuzgRUO0N</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>hoZsDsseA6B</v>
+        <v>JZ4Jt9JxsVh</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>p6zlpJrZzJV</v>
+        <v>pQ6jw6r59Op</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>kQCzFsC1eEU</v>
+        <v>YocjDGUCP18</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>cTcbZ8ht1zi</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>r83aoS5wveR</v>
+        <v>dbn6GloPaRP</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>GjZAEBGomjW</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>KYC90zR9e6n</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>VvJv2JhRgLE</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>h0FivHWebim</v>
-      </c>
-      <c r="E15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F15" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>HrI5yNYmham</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v>GvYhMDZrNH9</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v>hOLM46Ckolu</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>WSZu4jpViok</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>NMmB1l6X07Y</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="93.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2642,281 +2805,142 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>KYC90zR9e6n</v>
+        <v>pQ6jw6r59Op</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>HrI5yNYmham</v>
+        <v>neIuzgRUO0N</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>E94X1H21okK</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E6w4iwPkaRM</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="B7" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
+        <v>WcRHBfw09Iq</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>WSZu4jpViok</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
+        <v>oaBx9hR7FFR</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="B10" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>FjfJIiULctQ</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>n2mZrxngMFR</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>ud3dbLWVafm</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>cTcbZ8ht1zi</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Custom form</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Sections</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v>No</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>kIfMNugiTgd</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>No</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>Vs7Bd0pHjS9</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2938,37 +2962,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>p6zlpJrZzJV</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>jTGq07MlmMp</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2997,23 +3007,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3042,44 +3052,44 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>hZvJeK3Imky</v>
+        <v>BigUFwCduUF</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>V7qvIqRNyhQ</v>
+        <v>y9n0wxeewlR</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3100,7 +3110,7 @@
         <v>COVID19 access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-04-24</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>DoYehxUvmwT</v>
@@ -3111,28 +3121,17 @@
         <v>COVID19 admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-21</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>w4iJeNKy9br</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID19 data capture</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>k8Fk0kuhOeK</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3157,13 +3156,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>who</v>
+        <v>covid19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2018-07-13</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>vUeLeQMSwhN</v>
+        <v>F0YhCM0Pi73</v>
       </c>
     </row>
   </sheetData>
@@ -3172,99 +3171,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Section name</v>
+        <v>Last updated</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>BF8373CGyyT</v>
+        <v>i9rpQqB3Hfh</v>
       </c>
     </row>
   </sheetData>
@@ -3273,254 +3209,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="77.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Data Set Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Data Set Section</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Section UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>Data Element</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>Data Element UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
-      </c>
-      <c r="E7" s="5" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>njg6PAh5gw6</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
-      </c>
-      <c r="E12" s="4" t="str">
-        <v>e1xTRwfWega</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>h34jPNnKkJK</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>RC7RG6mexD2</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
   </sheetData>
@@ -3529,16 +3320,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3568,13 +3359,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases tested</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID_19_CASES_TESTED</v>
+        <v>CV19_NEW_CONF_PROB_HW_CASES</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
@@ -3583,136 +3374,136 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>SU1j9CmCuW9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Confirmed cases by transmission classification</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID_19_CONFIRMED_CASES_BY_TC</v>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>bmbNyNoJcXP</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>New cases hospitalised</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID_19_NEW_CASES_HOSPITALISED</v>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>default</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>rBw83gVQLHK</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - New cases treated</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>New cases treated</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID_19_NEW_CASES_TREATED</v>
+        <v>CV19_NEW_CONF_PROB_HW_DEATHS</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>DI9JgEJ3t8v</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>New confirmed cases (sex/age)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID_19_NEW_CONFIRMED_CASES</v>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>fJ7Qi1zcdAR</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>New deaths (sex/age)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID_19_NEW_DEATHS</v>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>cW0odY9vhrd</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New Suspected cases (sex/age)</v>
+        <v>New Probable Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID_19_NEW_SUSPECTED_CASES</v>
+        <v>CV19_NEW_PROB_CASES</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -3721,21 +3512,21 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>VnkErE22ELJ</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Recovered cases (sex/age)</v>
+        <v>New Probable Deaths</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID_19_RECOVERED_CASES</v>
+        <v>CV19_NEW_PROB_DEATHS</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -3744,44 +3535,44 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G9" s="5" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>N59eghaBpM7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Suspected cases by transmission classification</v>
+        <v>Tested</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID_19_SUSPECTED_CASES_BY_TC</v>
+        <v>CV19_TESTED</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
       </c>
       <c r="E10" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>E1pXvzyZzKB</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>COVID_19_TP_CLUSTER_CASES</v>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="D11" s="5" t="str">
         <v/>
@@ -3790,21 +3581,21 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>e1xTRwfWega</v>
+        <v>pZtyMNtYPLM</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern (Community  cases)</v>
+        <v>Transmission Classification</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID_19_TP_COMMUNITY_CASES</v>
+        <v>CV19_TRANS_CLASS</v>
       </c>
       <c r="D12" s="4" t="str">
         <v/>
@@ -3813,56 +3604,10 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>RC7RG6mexD2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID_19_TP_NO_CASES</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>default</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <v>njg6PAh5gw6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>COVID_19_TP_SPORADIC_CASES</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>default</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G14" s="4" t="str">
-        <v>h34jPNnKkJK</v>
+        <v>sWCFbUawFDa</v>
       </c>
     </row>
   </sheetData>
@@ -3871,13 +3616,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3893,7 +3638,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
     <row r="3">
@@ -3901,7 +3646,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
@@ -3909,7 +3654,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
@@ -3917,7 +3662,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="6">
@@ -3925,7 +3670,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="7">
@@ -3933,7 +3678,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="8">
@@ -3941,7 +3686,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="9">
@@ -3949,7 +3694,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="10">
@@ -3957,7 +3702,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="11">
@@ -3965,7 +3710,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="12">
@@ -3973,23 +3718,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
   </sheetData>
@@ -3998,15 +3727,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4028,13 +3757,13 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>o3OiZXHwBzY</v>
+        <v>UPxdJOxz2I7</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Age (COVID-19); Sex</v>
+        <v>Age (COVID19); Sex (with unknown)</v>
       </c>
     </row>
     <row r="3">
@@ -4042,41 +3771,13 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2017-05-28</v>
+        <v>2020-05-11</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bjDvmb4bfuf</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>default</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>FGDN1aBqJnt</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>sRwqVdFcBat</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
       </c>
     </row>
   </sheetData>
@@ -4085,15 +3786,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="126.7109375" customWidth="1"/>
+    <col min="4" max="4" width="176.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4112,16 +3813,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age (COVID-19)</v>
+        <v>Age (COVID19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>prZlmHqhxLO</v>
+        <v>RrZWSJ6CsLs</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>0-4 years; 5-14 years; 15-24 years; 25-34 years; 35-44 years; 45-54 years; 55-64 years; 65-74 years; 75-84 years; ≥ 85 years</v>
+        <v>0-4 years; 5-9 years; 10-14 years; 15-19 years; 20-29 years; 30-39 years; 40-49 years; 50-59 years; 60-64 years; 65-69 years; 70-74 years; 75-79 years; 80+ years; Unknown age</v>
       </c>
     </row>
     <row r="3">
@@ -4129,7 +3830,7 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>GLevLNI9wkl</v>
@@ -4140,44 +3841,16 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Sex</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-22</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>FRwO58KwwJt</v>
+        <v>b7peexUktxt</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Male; Female</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>v1atVR1HnCr</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Imported; Known Cluster; Community transmission; Unknown Classification</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>PWWzA79GcCG</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>Mechanical ventilation; ECMO; Admitted in intensive care unit (ICU)</v>
+        <v>Male; Female; Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -4186,12 +3859,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4209,13 +3882,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years</v>
+        <v>0-14 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2019-07-03</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>uueCp2RIGCJ</v>
+        <v>IoqDBYr0rH5</v>
       </c>
     </row>
     <row r="3">
@@ -4223,7 +3896,7 @@
         <v>0-4 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>UPvKbcqTEY3</v>
@@ -4231,255 +3904,189 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>ls9vGYWbvwG</v>
+        <v>ftXCKvbuGgj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>15-49 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jqg45gLQRYI</v>
+        <v>dENFBee17Oi</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>2-4 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>jxOEQ4Ss4bM</v>
+        <v>GERCWxK3mvz</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>25-34 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>O6UJSfL4psp</v>
+        <v>bY3NyagrzeD</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>35-44 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>utyLRFta4ie</v>
+        <v>tTmsWzvoEUv</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>45-54 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>nkQw9lhkbGV</v>
+        <v>J205eXYNH7q</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>5-14 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>pa0cY66MrG6</v>
+        <v>BOCPEdURsYX</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>50-64 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Yl34dHOPpZ0</v>
+        <v>TEBfAmuOSJk</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>55-64 years</v>
+        <v>65-69 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Lo1gxiS8zap</v>
+        <v>gHA96noC0iO</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>65-74 years</v>
+        <v>70-74 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AlUYlzoMVvN</v>
+        <v>Po7T5dd3tQs</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>65-79 years</v>
+        <v>75-79 years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>ZPzdstvH08a</v>
+        <v>xWXUBYNycnE</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>75-84 years</v>
+        <v>80+ years</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>R4m7KraS4aZ</v>
+        <v>c2hLbh0drQI</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>default</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2018-05-30</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>zUAhtH6iiyz</v>
+        <v>xYerKDKCefk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>hH4LYNplIeA</v>
+        <v>FFA9e1yIXCT</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>default</v>
+        <v>Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2018-05-30</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>xYerKDKCefk</v>
+        <v>MP15bHaQh2x</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>ECMO</v>
+        <v>Unknown age</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>mg1cBsgdqHC</v>
+        <v>WNPpyVkVaL3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>Female</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>FFA9e1yIXCT</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="str">
-        <v>Imported</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>y8TxHRrY1eN</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="str">
-        <v>Known Cluster</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C22" s="4" t="str">
-        <v>LIRv9sIHNOD</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="str">
-        <v>Male</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <v>MP15bHaQh2x</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <v>qoxRSWYj9cB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <v>YfLFBoAcjE2</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <v>F3RlEj6nnR3</v>
+        <v>kuP5EmQRFke</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add package for D2.32
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -16,16 +16,21 @@
     <sheet name="categoryOptionGroupSets" sheetId="11" r:id="rId11"/>
     <sheet name="categoryOptionGroups" sheetId="12" r:id="rId12"/>
     <sheet name="categoryOptionGroupsBySet" sheetId="13" r:id="rId13"/>
-    <sheet name="indicatorGroups" sheetId="14" r:id="rId14"/>
-    <sheet name="indicators" sheetId="15" r:id="rId15"/>
-    <sheet name="indicatorTypes" sheetId="16" r:id="rId16"/>
-    <sheet name="dashboards" sheetId="17" r:id="rId17"/>
-    <sheet name="dashboardItems" sheetId="18" r:id="rId18"/>
-    <sheet name="charts" sheetId="19" r:id="rId19"/>
-    <sheet name="reportTables" sheetId="20" r:id="rId20"/>
-    <sheet name="maps" sheetId="21" r:id="rId21"/>
-    <sheet name="userGroups" sheetId="22" r:id="rId22"/>
-    <sheet name="users" sheetId="23" r:id="rId23"/>
+    <sheet name="optionSets" sheetId="14" r:id="rId14"/>
+    <sheet name="options" sheetId="15" r:id="rId15"/>
+    <sheet name="validationRules" sheetId="16" r:id="rId16"/>
+    <sheet name="validationRuleGroups" sheetId="17" r:id="rId17"/>
+    <sheet name="validationRules by group" sheetId="18" r:id="rId18"/>
+    <sheet name="indicatorGroups" sheetId="19" r:id="rId19"/>
+    <sheet name="indicators" sheetId="20" r:id="rId20"/>
+    <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
+    <sheet name="dashboards" sheetId="22" r:id="rId22"/>
+    <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
+    <sheet name="maps" sheetId="26" r:id="rId26"/>
+    <sheet name="userGroups" sheetId="27" r:id="rId27"/>
+    <sheet name="users" sheetId="28" r:id="rId28"/>
   </sheets>
 </workbook>
 </file>
@@ -441,7 +446,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,7 +470,7 @@
         <v>Type</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>AGG</v>
+        <v>COMPLETE</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +478,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COMPLETE</v>
+        <v>V2.0</v>
       </c>
     </row>
     <row r="5">
@@ -481,7 +486,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>V1.0.1</v>
+        <v>DHIS2.32</v>
       </c>
     </row>
     <row r="6">
@@ -489,7 +494,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>DHIS2.32</v>
+        <v>2020-10-12T14:36</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +502,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID19_AGG_COMPLETE_V1.0.1_DHIS2.32_2020-03-27T08:25</v>
+        <v>COVID19_COMPLETE_V2.0_DHIS2.32_2020-10-12T14:36</v>
       </c>
     </row>
   </sheetData>
@@ -506,12 +511,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -529,420 +534,497 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years, Female</v>
+        <v>0-4 years, Female</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>h72VZMAIXNp</v>
+        <v>X7SGUlfmJa5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>0-1 years, Male</v>
+        <v>0-4 years, Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>NZkmbtZAFtN</v>
+        <v>d1XzGx028Z8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>0-4 years, Female</v>
+        <v>0-4 years, Unknown Sex</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>JzrkRqzvWhH</v>
+        <v>Ter1Z3EGkQM</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>0-4 years, Male</v>
+        <v>10-14 years, Female</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jQqLIn3xasU</v>
+        <v>vvpjmqp0psR</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>15-24 years, Female</v>
+        <v>10-14 years, Male</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>gPWH4piZwC0</v>
+        <v>SV1RvPdmAkj</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>15-24 years, Male</v>
+        <v>10-14 years, Unknown Sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>uhLnCuMwCGm</v>
+        <v>XUXU9zyHXN9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>15-49 years, Female</v>
+        <v>15-19 years, Female</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>sFJsKLHLBFj</v>
+        <v>F9pPSHdgzwj</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>15-49 years, Male</v>
+        <v>15-19 years, Male</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>lIqSozdCr27</v>
+        <v>sx3u16x80nV</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>2-4 years, Female</v>
+        <v>15-19 years, Unknown Sex</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>H9SWzT8B10p</v>
+        <v>CTWSo1P4qyZ</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>2-4 years, Male</v>
+        <v>20-29 years, Female</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>gMDoZ8IxLFd</v>
+        <v>SIxMfxXNBVo</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>25-34 years, Female</v>
+        <v>20-29 years, Male</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>NZ10jDzwugk</v>
+        <v>bB5hQrGwaD1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>25-34 years, Male</v>
+        <v>20-29 years, Unknown Sex</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AXgnJb5b1Je</v>
+        <v>EjYC7RAtkkQ</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>35-44 years, Female</v>
+        <v>30-39 years, Female</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>FWxLSWmBfd0</v>
+        <v>GiRwR3FD86i</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>35-44 years, Male</v>
+        <v>30-39 years, Male</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>RQChXxsEGmX</v>
+        <v>S17lTK4VVeE</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>45-54 years, Female</v>
+        <v>30-39 years, Unknown Sex</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>VvdznDS1Jcv</v>
+        <v>bAO3xBqTyUk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>45-54 years, Male</v>
+        <v>40-49 years, Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>s8mcd0VkZjn</v>
+        <v>JepUukzD91g</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>5-14 years, Female</v>
+        <v>40-49 years, Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>aIDylQ6ka3n</v>
+        <v>MysvJzZ0ADY</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>5-14 years, Male</v>
+        <v>40-49 years, Unknown Sex</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>bMkvQ4PSTz3</v>
+        <v>ejldVLyrIy7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>50-64 years, Female</v>
+        <v>5-9 years, Female</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>E03CigZ4AM9</v>
+        <v>g5XAclU6mWm</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>50-64 years, Male</v>
+        <v>5-9 years, Male</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Tjy4Mc08yCX</v>
+        <v>bm2siOxEk6w</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>55-64 years, Female</v>
+        <v>5-9 years, Unknown Sex</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>kz9PKqMwjE9</v>
+        <v>S7DctIRHOH4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>55-64 years, Male</v>
+        <v>50-59 years, Female</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>ZTM6ooK5E4V</v>
+        <v>cfJ88kcKfs2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>65-74 years, Female</v>
+        <v>50-59 years, Male</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>L9lGoMl4PWJ</v>
+        <v>Hqno1sfL72D</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>65-74 years, Male</v>
+        <v>50-59 years, Unknown Sex</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>KLFLwpmZLYl</v>
+        <v>nux1VokaZmF</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>65-79 years, Female</v>
+        <v>60-64 years, Female</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>IdLfgkfPvX6</v>
+        <v>ABYB6U68hMU</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>65-79 years, Male</v>
+        <v>60-64 years, Male</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>JtGMAcD0Btm</v>
+        <v>vsG6W671YoN</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>75-84 years, Female</v>
+        <v>60-64 years, Unknown Sex</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>lMo9HzUDdeM</v>
+        <v>YUMOQHnN8pn</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>75-84 years, Male</v>
+        <v>65-69 years, Female</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>F9mySvLgUiB</v>
+        <v>SZ9ccMeGlS6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years, Male</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>FFMPsVh7sxb</v>
+        <v>H0mzaMCOq2e</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>Community transmission</v>
+        <v>65-69 years, Unknown Sex</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>p2ahkO4fbJ9</v>
+        <v>llEP85jmlnN</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>default</v>
+        <v>70-74 years, Female</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>HllvX50cXC0</v>
+        <v>D0g8d1tsNnv</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>ECMO</v>
+        <v>70-74 years, Male</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>cEjvma5H9Il</v>
+        <v>oEsLwo2ah7U</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>Imported</v>
+        <v>70-74 years, Unknown Sex</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>S32sBnGUfwN</v>
+        <v>JC2mJwkcXQ2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>75-79 years, Female</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>tTh6wRIEtFa</v>
+        <v>Lic97hqxsNP</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>Mechanical ventilation</v>
+        <v>75-79 years, Male</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>hJjSk6eIuDt</v>
+        <v>PgmLRiqPKgd</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>75-79 years, Unknown Sex</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>lWjjUr72APP</v>
+        <v>byqkmEDJ42u</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>≥ 85 years, Female</v>
+        <v>80+ years, Female</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>cO1vAjqfkUz</v>
+        <v>RzvnXjQu1cm</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>≥ 85 years, Male</v>
+        <v>80+ years, Male</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>vJ6enc1w0lu</v>
+        <v>zjOFUnSP4cf</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>80+ years, Unknown Sex</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>P6caJBLkaq9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>default</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>2020-03-26</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>HllvX50cXC0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>Female, 0-14 years</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>GHDbaPccoPh</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="str">
+        <v>Male, 0-14 years</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <v>KMTXoNkoiAc</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="str">
+        <v>Unknown age, Female</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <v>w1W0eGecUME</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="str">
+        <v>Unknown age, Male</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <v>BAJrVjxh8K9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="str">
+        <v>Unknown age, Unknown Sex</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <v>meAnvpEpz8M</v>
       </c>
     </row>
   </sheetData>
@@ -951,12 +1033,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -974,46 +1056,24 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>GaGDeErYt4e</v>
+        <v>nd6HGxbW3D5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>CMrvZp5rmoC</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>kJ82l0tJUoe</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>VSS1t1HOSWD</v>
+        <v>XxEFGdwxOJ0</v>
       </c>
     </row>
   </sheetData>
@@ -1022,13 +1082,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1052,10 +1112,10 @@
         <v>0-4 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>0-4 years</v>
+        <v>0-4 y</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yuathFHLjNe</v>
@@ -1063,254 +1123,212 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>15-24 y</v>
+        <v>10-14 y</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>L7gAblMOZKs</v>
+        <v>RoYZKp6iDnH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>25-34 y</v>
+        <v>15-19 y</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>cRskhJQLr4J</v>
+        <v>qiaJA9sMzj2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>35-44 y</v>
+        <v>20-29 y</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>KkZHYvn7Zor</v>
+        <v>p84eezwJhMd</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>45-54 y</v>
+        <v>30-39 y</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>y5yT8JF4uCA</v>
+        <v>u87kL0SUYZa</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>5-14 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>5-14 y</v>
+        <v>40-49 y</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>V9t81g7Wspa</v>
+        <v>nuU9qXctcQE</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 y</v>
+        <v>5-9 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>QllZ8PveFCQ</v>
+        <v>Mcv3dvoK2iM</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74  y</v>
+        <v>50-59 y</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>Y4rNex59t8s</v>
+        <v>IpuKFEXhtUJ</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84  y</v>
+        <v>60-64 y</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>SFZ9S9XHquk</v>
+        <v>JrQqLgsGgFr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>ICU</v>
+        <v>65-69 y</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>XDghoAFhOHg</v>
+        <v>Bap549vCg8U</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 y</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>SKB3wBAOrC2</v>
+        <v>t1JMgMVyoac</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 y</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>QkutHMU0t2V</v>
+        <v>FplLHwIitbU</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ y</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>bqoVhX2RfG4</v>
+        <v>v1e6orGTL3f</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>L8hy5JsqneC</v>
+        <v>bqoVhX2RfG4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>C7gopCwNhoa</v>
+        <v>EVYKU2fIc6G</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Male</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Male</v>
+        <v>Unk Sex</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>EVYKU2fIc6G</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>MV</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>QLONA1SnwU5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <v>QRRRfUrxJs0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>≥ 85 y</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>GL19QsdIgIu</v>
+        <v>SZJNeRyrh22</v>
       </c>
     </row>
   </sheetData>
@@ -1319,13 +1337,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1338,7 +1356,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>0-4 years</v>
@@ -1346,146 +1364,130 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>5-14 years</v>
+        <v>5-9 years</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>40-49 years</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>≥ 85 years</v>
+        <v>65-69 years</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Female</v>
+        <v>70-74 years</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Male</v>
+        <v>75-79 years</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Imported</v>
+        <v>80+ years</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>Male</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>ECMO</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -1499,7 +1501,321 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Options</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Transmission Classification</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>No cases; Sporadic; Clusters; Community</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Option set UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>NzPq5MlxCmh</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>Clusters</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>CLUSTERS</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>zUdhwKZdpT8</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Community</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>COMMUNITY</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>mF5r1p7sKcq</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>No cases</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>NO_CASES</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>AXl3Z9rLjLi</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>Sporadic</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>SPORADIC</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Instruction</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Left side</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Operator</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Right side</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>New Cases hospitalised should be less than or equal to All new cases reported</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>New Cases hospitalised</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>All New Cases</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>bO8rXNzj0iR</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Test with PCR should be less than or equal to tested</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>Tested with PCR</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>Tested</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <v>gZwUbrTOa0g</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>WY7h5pKok2I</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Validation Rule Group</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Validation Rule</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1521,36 +1837,99 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19</v>
+        <v>COVID19</v>
       </c>
       <c r="B2" s="4" t="str">
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Property</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Name:</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>Custom form:</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Sections:</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>UID:</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>uKtOZwDnIpM</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="153.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
@@ -1590,16 +1969,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>zUcGi0Y384Y</v>
+        <v>ZTklbd8JtLn</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - Active cases</v>
+        <v>COVID19 - Active cases</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Active cases</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v/>
+        <v>CV19_ACTIVE_CASES</v>
       </c>
       <c r="E2" s="4" t="str">
         <v/>
@@ -1614,94 +1993,94 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>kJoSHTinHGa</v>
+        <v>LeNVLm6SL1x</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - All cases</v>
+        <v>COVID19 - Case fatality rate (%)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>All cases</v>
+        <v>Case Fatality rate (%)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE</v>
       </c>
       <c r="E3" s="5" t="str">
         <v/>
       </c>
       <c r="F3" s="5" t="str">
-        <v>All cases</v>
+        <v>Death (Confirmed + Probable)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J3" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>dXAhOKiim1x</v>
+        <v>NP88sGFKpCQ</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Case Fatality rate (%)</v>
+        <v>COVID19 - Case fatality rate among HW (%)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Case Fatality rate (%)</v>
+        <v>Case fatality rate HW (%)</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE_HW</v>
       </c>
       <c r="E4" s="4" t="str">
         <v/>
       </c>
       <c r="F4" s="4" t="str">
-        <v>Deaths Reported</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="H4" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J4" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>fK1b7O6CuBV</v>
+        <v>VJHMO9gHkV5</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Cases treated by mechanical ventilation, ECMO or ICU</v>
+        <v>COVID19 - Closed cases</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Cases treated by type</v>
+        <v>Closed cases</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v/>
+        <v>CV19_CLOSED_CASES</v>
       </c>
       <c r="E5" s="5" t="str">
         <v/>
       </c>
       <c r="F5" s="5" t="str">
-        <v>Number of suspected cases that received mechanical ventilation, ECMO or admitted into intensive care unit</v>
+        <v>Closed cases</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>1</v>
@@ -1710,30 +2089,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J5" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>S3Ty19GEaqn</v>
+        <v>TmKNBHtBx6D</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Closed cases</v>
+        <v>COVID19 - New Confirmed cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Closed cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="E6" s="4" t="str">
         <v/>
       </c>
       <c r="F6" s="4" t="str">
-        <v>Active Cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>1</v>
@@ -1742,30 +2121,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J6" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>ocBlGrHZy6Q</v>
+        <v>yzyWxXoSCny</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Confirmed cases</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="E7" s="5" t="str">
         <v/>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Suspected cases that were confirmed through laboratory testing (multiple lab tests may be conducted; this indicator assumes that the last test result).</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>1</v>
@@ -1774,30 +2153,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J7" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zozhRzInMZm</v>
+        <v>U89bOzPbFyA</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by Transmission Classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="E8" s="4" t="str">
         <v/>
       </c>
       <c r="F8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>1</v>
@@ -1806,30 +2185,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J8" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>r2VxAVW1IEy</v>
+        <v>DnleIypnqxJ</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - Deaths</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Deaths</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="E9" s="5" t="str">
         <v/>
       </c>
       <c r="F9" s="5" t="str">
-        <v>COVID-19 related deaths (deaths recorded among all suspected cases)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -1838,158 +2217,158 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J9" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>BmW2IAaxIBe</v>
+        <v>C6A59SObXV6</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - Hospitalised Cases</v>
+        <v>COVID19 - Positivity rate (%)</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Hospitalised Cases</v>
+        <v>Positivity rate (%)</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v/>
+        <v>CV19_POSITIVITY_RATE</v>
       </c>
       <c r="E10" s="4" t="str">
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <v>Number of suspected or confirmed or probable cases that were admitted into hospital</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>1</v>
+        <v>Tested</v>
       </c>
       <c r="H10" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J10" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>jHzx1zXeHzV</v>
+        <v>x6IelBioEX1</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Proportion of males among confirmed cases (%)</v>
+        <v>COVID19 - Proportion of HW amongst reported cases (%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Proportion of males among confirmed cases (%)</v>
+        <v>HW among confirmed cases (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v/>
+        <v>CV19_%_HW_AMONGST_REPORTED_CASES</v>
       </c>
       <c r="E11" s="5" t="str">
         <v/>
       </c>
       <c r="F11" s="5" t="str">
-        <v>Males among confirmed cases</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="H11" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J11" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>UF7s1t1v6KG</v>
+        <v>cJZS7kSFFGl</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - Proportion of males among deaths(%)</v>
+        <v>COVID19 - Proportion of PCR tests (%)</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Proportion of males among deaths (%)</v>
+        <v>Proportion of PCR tests</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v/>
+        <v>CV19_%_PCR_TESTS</v>
       </c>
       <c r="E12" s="4" t="str">
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <v>Males among deaths</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>Deaths</v>
+        <v>Tested</v>
       </c>
       <c r="H12" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J12" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>gYt2GEAdCJK</v>
+        <v>K2JqazsxhvP</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Recovery rate (%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Recovery rate (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v/>
+        <v>CV19_RECOVERY_RATE</v>
       </c>
       <c r="E13" s="5" t="str">
         <v/>
       </c>
       <c r="F13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J13" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>JpRDu51rbg5</v>
+        <v>pxqFjCNLkzD</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v/>
+        <v>CV19_TESTED</v>
       </c>
       <c r="E14" s="4" t="str">
         <v/>
       </c>
       <c r="F14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>1</v>
@@ -1998,30 +2377,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J14" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>vECy4BgZqRF</v>
+        <v>jgyO0rV708H</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (No cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v/>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="E15" s="5" t="str">
         <v/>
       </c>
       <c r="F15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>1</v>
@@ -2030,113 +2409,17 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J15" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>GszrLGBvHhg</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="G16" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>PkGdfHQyWWH</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>COVID-19 - Recovered cases</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>Recovered cases</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>Number of cases that are recovered.</v>
-      </c>
-      <c r="G17" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I17" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J17" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>dsho3rAaUkr</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>COVID-19 - Recovery rate (%)</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>Case Recovery rate</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>Cases Recovered</v>
-      </c>
-      <c r="G18" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
-      </c>
-      <c r="H18" s="4" t="str">
-        <v>Percentage</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J18" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2171,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2018-01-16</v>
+        <v>2020-09-09</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>kHy61PbChXr</v>
@@ -2195,14 +2478,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2220,29 +2503,29 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>04. COVID-19 Surveillance (Aggregate)</v>
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="93.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -2270,356 +2553,236 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>ud3dbLWVafm</v>
+        <v>jTGq07MlmMp</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>ZcYLgBQrhgu</v>
+        <v>btrkVNdRwnO</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>n2mZrxngMFR</v>
+        <v>oaBx9hR7FFR</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>nIVBxZaZ8Gd</v>
+        <v>jmn7HoMmBHC</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>FjfJIiULctQ</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>lIAZDq6H4dF</v>
+        <v>JNHOYQEIN3V</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>o9HS22p81W0</v>
+        <v>P7syfXG9dNm</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>E6w4iwPkaRM</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>YzYCsOsZDz2</v>
+        <v>IeZQZcgmAfV</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>dFmHVADG2t5</v>
+        <v>KWM5EsM8hYR</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>WcRHBfw09Iq</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>cSmHf59IIs5</v>
+        <v>qTkvVnIP5Ri</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E94X1H21okK</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>kz9Z0mKZQbN</v>
+        <v>KMsy5gLLUWr</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>neIuzgRUO0N</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>hoZsDsseA6B</v>
+        <v>JZ4Jt9JxsVh</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>p6zlpJrZzJV</v>
+        <v>pQ6jw6r59Op</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>kQCzFsC1eEU</v>
+        <v>YocjDGUCP18</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>cTcbZ8ht1zi</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>r83aoS5wveR</v>
+        <v>dbn6GloPaRP</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>GjZAEBGomjW</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>KYC90zR9e6n</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>VvJv2JhRgLE</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>h0FivHWebim</v>
-      </c>
-      <c r="E15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F15" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>HrI5yNYmham</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v>GvYhMDZrNH9</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v>hOLM46Ckolu</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>WSZu4jpViok</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>NMmB1l6X07Y</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="93.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2641,281 +2804,142 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>KYC90zR9e6n</v>
+        <v>pQ6jw6r59Op</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>HrI5yNYmham</v>
+        <v>neIuzgRUO0N</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>E94X1H21okK</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E6w4iwPkaRM</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="B7" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
+        <v>WcRHBfw09Iq</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>WSZu4jpViok</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
+        <v>oaBx9hR7FFR</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="B10" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>FjfJIiULctQ</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>n2mZrxngMFR</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>ud3dbLWVafm</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>cTcbZ8ht1zi</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Custom form</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Sections</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v>No</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>kIfMNugiTgd</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>No</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>Vs7Bd0pHjS9</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2937,37 +2961,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>p6zlpJrZzJV</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>jTGq07MlmMp</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2996,30 +3006,30 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3040,7 +3050,7 @@
         <v>COVID19 access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-04-24</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>DoYehxUvmwT</v>
@@ -3051,28 +3061,17 @@
         <v>COVID19 admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-21</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>w4iJeNKy9br</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID19 data capture</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>k8Fk0kuhOeK</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3097,13 +3096,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>who</v>
+        <v>covid19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2018-07-13</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>vUeLeQMSwhN</v>
+        <v>F0YhCM0Pi73</v>
       </c>
     </row>
   </sheetData>
@@ -3112,99 +3111,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Section name</v>
+        <v>Last updated</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>BF8373CGyyT</v>
+        <v>i9rpQqB3Hfh</v>
       </c>
     </row>
   </sheetData>
@@ -3213,254 +3149,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="77.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Data Set Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Data Set Section</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Section UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>Data Element</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>Data Element UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
-      </c>
-      <c r="E7" s="5" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>njg6PAh5gw6</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
-      </c>
-      <c r="E12" s="4" t="str">
-        <v>e1xTRwfWega</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>h34jPNnKkJK</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>RC7RG6mexD2</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
   </sheetData>
@@ -3469,16 +3260,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3508,13 +3299,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases tested</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID_19_CASES_TESTED</v>
+        <v>CV19_NEW_CONF_PROB_HW_CASES</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
@@ -3523,136 +3314,136 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>SU1j9CmCuW9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Confirmed cases by transmission classification</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID_19_CONFIRMED_CASES_BY_TC</v>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>bmbNyNoJcXP</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>New cases hospitalised</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID_19_NEW_CASES_HOSPITALISED</v>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>default</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>rBw83gVQLHK</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - New cases treated</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>New cases treated</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID_19_NEW_CASES_TREATED</v>
+        <v>CV19_NEW_CONF_PROB_HW_DEATHS</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>DI9JgEJ3t8v</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>New confirmed cases (sex/age)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID_19_NEW_CONFIRMED_CASES</v>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>fJ7Qi1zcdAR</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>New deaths (sex/age)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID_19_NEW_DEATHS</v>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>cW0odY9vhrd</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New Suspected cases (sex/age)</v>
+        <v>New Probable Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID_19_NEW_SUSPECTED_CASES</v>
+        <v>CV19_NEW_PROB_CASES</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -3661,21 +3452,21 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>VnkErE22ELJ</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Recovered cases (sex/age)</v>
+        <v>New Probable Deaths</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID_19_RECOVERED_CASES</v>
+        <v>CV19_NEW_PROB_DEATHS</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -3684,44 +3475,44 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G9" s="5" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>N59eghaBpM7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Suspected cases by transmission classification</v>
+        <v>Tested</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID_19_SUSPECTED_CASES_BY_TC</v>
+        <v>CV19_TESTED</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
       </c>
       <c r="E10" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>E1pXvzyZzKB</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>COVID_19_TP_CLUSTER_CASES</v>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="D11" s="5" t="str">
         <v/>
@@ -3730,21 +3521,21 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>e1xTRwfWega</v>
+        <v>pZtyMNtYPLM</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern (Community  cases)</v>
+        <v>Transmission Classification</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID_19_TP_COMMUNITY_CASES</v>
+        <v>CV19_TRANS_CLASS</v>
       </c>
       <c r="D12" s="4" t="str">
         <v/>
@@ -3753,56 +3544,10 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>RC7RG6mexD2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID_19_TP_NO_CASES</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>default</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <v>njg6PAh5gw6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>COVID_19_TP_SPORADIC_CASES</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>default</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G14" s="4" t="str">
-        <v>h34jPNnKkJK</v>
+        <v>sWCFbUawFDa</v>
       </c>
     </row>
   </sheetData>
@@ -3811,13 +3556,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3833,7 +3578,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
     <row r="3">
@@ -3841,7 +3586,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
@@ -3849,7 +3594,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
@@ -3857,7 +3602,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="6">
@@ -3865,7 +3610,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="7">
@@ -3873,7 +3618,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="8">
@@ -3881,7 +3626,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="9">
@@ -3889,7 +3634,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="10">
@@ -3897,7 +3642,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="11">
@@ -3905,7 +3650,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="12">
@@ -3913,23 +3658,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
   </sheetData>
@@ -3938,15 +3667,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3968,13 +3697,13 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>o3OiZXHwBzY</v>
+        <v>UPxdJOxz2I7</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Age (COVID-19); Sex</v>
+        <v>Age (COVID19); Sex (with unknown)</v>
       </c>
     </row>
     <row r="3">
@@ -3982,41 +3711,13 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2017-05-28</v>
+        <v>2020-05-11</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bjDvmb4bfuf</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>default</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>FGDN1aBqJnt</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>sRwqVdFcBat</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
       </c>
     </row>
   </sheetData>
@@ -4025,15 +3726,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="126.7109375" customWidth="1"/>
+    <col min="4" max="4" width="176.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4052,16 +3753,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age (COVID-19)</v>
+        <v>Age (COVID19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>prZlmHqhxLO</v>
+        <v>RrZWSJ6CsLs</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>0-4 years; 5-14 years; 15-24 years; 25-34 years; 35-44 years; 45-54 years; 55-64 years; 65-74 years; 75-84 years; ≥ 85 years</v>
+        <v>0-4 years; 5-9 years; 10-14 years; 15-19 years; 20-29 years; 30-39 years; 40-49 years; 50-59 years; 60-64 years; 65-69 years; 70-74 years; 75-79 years; 80+ years; Unknown age</v>
       </c>
     </row>
     <row r="3">
@@ -4069,7 +3770,7 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>GLevLNI9wkl</v>
@@ -4080,44 +3781,16 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Sex</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-22</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>FRwO58KwwJt</v>
+        <v>b7peexUktxt</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Male; Female</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>v1atVR1HnCr</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Imported; Known Cluster; Community transmission; Unknown Classification</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>PWWzA79GcCG</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>Mechanical ventilation; ECMO; Admitted in intensive care unit (ICU)</v>
+        <v>Male; Female; Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -4126,12 +3799,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4149,13 +3822,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years</v>
+        <v>0-14 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2019-07-03</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>uueCp2RIGCJ</v>
+        <v>IoqDBYr0rH5</v>
       </c>
     </row>
     <row r="3">
@@ -4163,7 +3836,7 @@
         <v>0-4 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>UPvKbcqTEY3</v>
@@ -4171,255 +3844,189 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>ls9vGYWbvwG</v>
+        <v>ftXCKvbuGgj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>15-49 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jqg45gLQRYI</v>
+        <v>dENFBee17Oi</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>2-4 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>jxOEQ4Ss4bM</v>
+        <v>GERCWxK3mvz</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>25-34 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>O6UJSfL4psp</v>
+        <v>bY3NyagrzeD</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>35-44 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>utyLRFta4ie</v>
+        <v>tTmsWzvoEUv</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>45-54 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>nkQw9lhkbGV</v>
+        <v>J205eXYNH7q</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>5-14 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>pa0cY66MrG6</v>
+        <v>BOCPEdURsYX</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>50-64 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Yl34dHOPpZ0</v>
+        <v>TEBfAmuOSJk</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>55-64 years</v>
+        <v>65-69 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Lo1gxiS8zap</v>
+        <v>gHA96noC0iO</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>65-74 years</v>
+        <v>70-74 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AlUYlzoMVvN</v>
+        <v>Po7T5dd3tQs</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>65-79 years</v>
+        <v>75-79 years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>ZPzdstvH08a</v>
+        <v>xWXUBYNycnE</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>75-84 years</v>
+        <v>80+ years</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>R4m7KraS4aZ</v>
+        <v>c2hLbh0drQI</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>default</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2018-05-30</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>zUAhtH6iiyz</v>
+        <v>xYerKDKCefk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>hH4LYNplIeA</v>
+        <v>FFA9e1yIXCT</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>default</v>
+        <v>Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2018-05-30</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>xYerKDKCefk</v>
+        <v>MP15bHaQh2x</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>ECMO</v>
+        <v>Unknown age</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>mg1cBsgdqHC</v>
+        <v>WNPpyVkVaL3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>Female</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>FFA9e1yIXCT</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="str">
-        <v>Imported</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>y8TxHRrY1eN</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="str">
-        <v>Known Cluster</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C22" s="4" t="str">
-        <v>LIRv9sIHNOD</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="str">
-        <v>Male</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <v>MP15bHaQh2x</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <v>qoxRSWYj9cB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <v>YfLFBoAcjE2</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <v>F3RlEj6nnR3</v>
+        <v>kuP5EmQRFke</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add package for D2.33
</commit_message>
<xml_diff>
--- a/complete/reference.xlsx
+++ b/complete/reference.xlsx
@@ -16,16 +16,21 @@
     <sheet name="categoryOptionGroupSets" sheetId="11" r:id="rId11"/>
     <sheet name="categoryOptionGroups" sheetId="12" r:id="rId12"/>
     <sheet name="categoryOptionGroupsBySet" sheetId="13" r:id="rId13"/>
-    <sheet name="indicatorGroups" sheetId="14" r:id="rId14"/>
-    <sheet name="indicators" sheetId="15" r:id="rId15"/>
-    <sheet name="indicatorTypes" sheetId="16" r:id="rId16"/>
-    <sheet name="dashboards" sheetId="17" r:id="rId17"/>
-    <sheet name="dashboardItems" sheetId="18" r:id="rId18"/>
-    <sheet name="charts" sheetId="19" r:id="rId19"/>
-    <sheet name="reportTables" sheetId="20" r:id="rId20"/>
-    <sheet name="maps" sheetId="21" r:id="rId21"/>
-    <sheet name="userGroups" sheetId="22" r:id="rId22"/>
-    <sheet name="users" sheetId="23" r:id="rId23"/>
+    <sheet name="optionSets" sheetId="14" r:id="rId14"/>
+    <sheet name="options" sheetId="15" r:id="rId15"/>
+    <sheet name="validationRules" sheetId="16" r:id="rId16"/>
+    <sheet name="validationRuleGroups" sheetId="17" r:id="rId17"/>
+    <sheet name="validationRules by group" sheetId="18" r:id="rId18"/>
+    <sheet name="indicatorGroups" sheetId="19" r:id="rId19"/>
+    <sheet name="indicators" sheetId="20" r:id="rId20"/>
+    <sheet name="indicatorTypes" sheetId="21" r:id="rId21"/>
+    <sheet name="dashboards" sheetId="22" r:id="rId22"/>
+    <sheet name="dashboardItems" sheetId="23" r:id="rId23"/>
+    <sheet name="charts" sheetId="24" r:id="rId24"/>
+    <sheet name="reportTables" sheetId="25" r:id="rId25"/>
+    <sheet name="maps" sheetId="26" r:id="rId26"/>
+    <sheet name="userGroups" sheetId="27" r:id="rId27"/>
+    <sheet name="users" sheetId="28" r:id="rId28"/>
   </sheets>
 </workbook>
 </file>
@@ -441,7 +446,7 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -465,7 +470,7 @@
         <v>Type</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>AGG</v>
+        <v>COMPLETE</v>
       </c>
     </row>
     <row r="4">
@@ -473,7 +478,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COMPLETE</v>
+        <v>V2.0</v>
       </c>
     </row>
     <row r="5">
@@ -481,7 +486,7 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>V1.0.1</v>
+        <v>DHIS2.33</v>
       </c>
     </row>
     <row r="6">
@@ -489,7 +494,7 @@
         <v>Created</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>DHIS2.33</v>
+        <v>2020-10-12T15:17</v>
       </c>
     </row>
     <row r="7">
@@ -497,7 +502,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID19_AGG_COMPLETE_V1.0.1_DHIS2.33_2020-03-27T08:25</v>
+        <v>COVID19_COMPLETE_V2.0_DHIS2.33_2020-10-12T15:17</v>
       </c>
     </row>
   </sheetData>
@@ -506,12 +511,12 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -529,420 +534,497 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years, Female</v>
+        <v>0-4 years, Female</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>h72VZMAIXNp</v>
+        <v>X7SGUlfmJa5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>0-1 years, Male</v>
+        <v>0-4 years, Male</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>NZkmbtZAFtN</v>
+        <v>d1XzGx028Z8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>0-4 years, Female</v>
+        <v>0-4 years, Unknown Sex</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>JzrkRqzvWhH</v>
+        <v>Ter1Z3EGkQM</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>0-4 years, Male</v>
+        <v>10-14 years, Female</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jQqLIn3xasU</v>
+        <v>vvpjmqp0psR</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>15-24 years, Female</v>
+        <v>10-14 years, Male</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>gPWH4piZwC0</v>
+        <v>SV1RvPdmAkj</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>15-24 years, Male</v>
+        <v>10-14 years, Unknown Sex</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>uhLnCuMwCGm</v>
+        <v>XUXU9zyHXN9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>15-49 years, Female</v>
+        <v>15-19 years, Female</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>sFJsKLHLBFj</v>
+        <v>F9pPSHdgzwj</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>15-49 years, Male</v>
+        <v>15-19 years, Male</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>lIqSozdCr27</v>
+        <v>sx3u16x80nV</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>2-4 years, Female</v>
+        <v>15-19 years, Unknown Sex</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>H9SWzT8B10p</v>
+        <v>CTWSo1P4qyZ</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>2-4 years, Male</v>
+        <v>20-29 years, Female</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>gMDoZ8IxLFd</v>
+        <v>SIxMfxXNBVo</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>25-34 years, Female</v>
+        <v>20-29 years, Male</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>NZ10jDzwugk</v>
+        <v>bB5hQrGwaD1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>25-34 years, Male</v>
+        <v>20-29 years, Unknown Sex</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AXgnJb5b1Je</v>
+        <v>EjYC7RAtkkQ</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>35-44 years, Female</v>
+        <v>30-39 years, Female</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>FWxLSWmBfd0</v>
+        <v>GiRwR3FD86i</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>35-44 years, Male</v>
+        <v>30-39 years, Male</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>RQChXxsEGmX</v>
+        <v>S17lTK4VVeE</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>45-54 years, Female</v>
+        <v>30-39 years, Unknown Sex</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>VvdznDS1Jcv</v>
+        <v>bAO3xBqTyUk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>45-54 years, Male</v>
+        <v>40-49 years, Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>s8mcd0VkZjn</v>
+        <v>JepUukzD91g</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>5-14 years, Female</v>
+        <v>40-49 years, Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>aIDylQ6ka3n</v>
+        <v>MysvJzZ0ADY</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>5-14 years, Male</v>
+        <v>40-49 years, Unknown Sex</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>bMkvQ4PSTz3</v>
+        <v>ejldVLyrIy7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>50-64 years, Female</v>
+        <v>5-9 years, Female</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>E03CigZ4AM9</v>
+        <v>g5XAclU6mWm</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>50-64 years, Male</v>
+        <v>5-9 years, Male</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Tjy4Mc08yCX</v>
+        <v>bm2siOxEk6w</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>55-64 years, Female</v>
+        <v>5-9 years, Unknown Sex</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>kz9PKqMwjE9</v>
+        <v>S7DctIRHOH4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>55-64 years, Male</v>
+        <v>50-59 years, Female</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>ZTM6ooK5E4V</v>
+        <v>cfJ88kcKfs2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>65-74 years, Female</v>
+        <v>50-59 years, Male</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>L9lGoMl4PWJ</v>
+        <v>Hqno1sfL72D</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>65-74 years, Male</v>
+        <v>50-59 years, Unknown Sex</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>KLFLwpmZLYl</v>
+        <v>nux1VokaZmF</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>65-79 years, Female</v>
+        <v>60-64 years, Female</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>IdLfgkfPvX6</v>
+        <v>ABYB6U68hMU</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>65-79 years, Male</v>
+        <v>60-64 years, Male</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>JtGMAcD0Btm</v>
+        <v>vsG6W671YoN</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>75-84 years, Female</v>
+        <v>60-64 years, Unknown Sex</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>lMo9HzUDdeM</v>
+        <v>YUMOQHnN8pn</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>75-84 years, Male</v>
+        <v>65-69 years, Female</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>F9mySvLgUiB</v>
+        <v>SZ9ccMeGlS6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years, Male</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>FFMPsVh7sxb</v>
+        <v>H0mzaMCOq2e</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>Community transmission</v>
+        <v>65-69 years, Unknown Sex</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>p2ahkO4fbJ9</v>
+        <v>llEP85jmlnN</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>default</v>
+        <v>70-74 years, Female</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>HllvX50cXC0</v>
+        <v>D0g8d1tsNnv</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>ECMO</v>
+        <v>70-74 years, Male</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>cEjvma5H9Il</v>
+        <v>oEsLwo2ah7U</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>Imported</v>
+        <v>70-74 years, Unknown Sex</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>S32sBnGUfwN</v>
+        <v>JC2mJwkcXQ2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>75-79 years, Female</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>tTh6wRIEtFa</v>
+        <v>Lic97hqxsNP</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>Mechanical ventilation</v>
+        <v>75-79 years, Male</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>hJjSk6eIuDt</v>
+        <v>PgmLRiqPKgd</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>75-79 years, Unknown Sex</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>lWjjUr72APP</v>
+        <v>byqkmEDJ42u</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>≥ 85 years, Female</v>
+        <v>80+ years, Female</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>cO1vAjqfkUz</v>
+        <v>RzvnXjQu1cm</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>≥ 85 years, Male</v>
+        <v>80+ years, Male</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>vJ6enc1w0lu</v>
+        <v>zjOFUnSP4cf</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="str">
+        <v>80+ years, Unknown Sex</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C40" s="4" t="str">
+        <v>P6caJBLkaq9</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="5" t="str">
+        <v>default</v>
+      </c>
+      <c r="B41" s="5" t="str">
+        <v>2020-03-26</v>
+      </c>
+      <c r="C41" s="5" t="str">
+        <v>HllvX50cXC0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="str">
+        <v>Female, 0-14 years</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C42" s="4" t="str">
+        <v>GHDbaPccoPh</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="5" t="str">
+        <v>Male, 0-14 years</v>
+      </c>
+      <c r="B43" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C43" s="5" t="str">
+        <v>KMTXoNkoiAc</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="str">
+        <v>Unknown age, Female</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C44" s="4" t="str">
+        <v>w1W0eGecUME</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="5" t="str">
+        <v>Unknown age, Male</v>
+      </c>
+      <c r="B45" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C45" s="5" t="str">
+        <v>BAJrVjxh8K9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="str">
+        <v>Unknown age, Unknown Sex</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C46" s="4" t="str">
+        <v>meAnvpEpz8M</v>
       </c>
     </row>
   </sheetData>
@@ -951,12 +1033,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -974,46 +1056,24 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>GaGDeErYt4e</v>
+        <v>nd6HGxbW3D5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>CMrvZp5rmoC</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>kJ82l0tJUoe</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>VSS1t1HOSWD</v>
+        <v>XxEFGdwxOJ0</v>
       </c>
     </row>
   </sheetData>
@@ -1022,13 +1082,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
@@ -1052,10 +1112,10 @@
         <v>0-4 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>0-4 years</v>
+        <v>0-4 y</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>yuathFHLjNe</v>
@@ -1063,254 +1123,212 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>15-24 y</v>
+        <v>10-14 y</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>L7gAblMOZKs</v>
+        <v>RoYZKp6iDnH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>25-34 y</v>
+        <v>15-19 y</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>cRskhJQLr4J</v>
+        <v>qiaJA9sMzj2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>35-44 y</v>
+        <v>20-29 y</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>KkZHYvn7Zor</v>
+        <v>p84eezwJhMd</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>45-54 y</v>
+        <v>30-39 y</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>y5yT8JF4uCA</v>
+        <v>u87kL0SUYZa</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>5-14 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>5-14 y</v>
+        <v>40-49 y</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>V9t81g7Wspa</v>
+        <v>nuU9qXctcQE</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 y</v>
+        <v>5-9 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2019-06-29</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>QllZ8PveFCQ</v>
+        <v>Mcv3dvoK2iM</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74  y</v>
+        <v>50-59 y</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>Y4rNex59t8s</v>
+        <v>IpuKFEXhtUJ</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84  y</v>
+        <v>60-64 y</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>SFZ9S9XHquk</v>
+        <v>JrQqLgsGgFr</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>65-69 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>ICU</v>
+        <v>65-69 y</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>XDghoAFhOHg</v>
+        <v>Bap549vCg8U</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Community transmission</v>
+        <v>70-74 y</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>SKB3wBAOrC2</v>
+        <v>t1JMgMVyoac</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>ECMO</v>
+        <v>75-79 y</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>QkutHMU0t2V</v>
+        <v>FplLHwIitbU</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Female</v>
+        <v>80+ y</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>bqoVhX2RfG4</v>
+        <v>v1e6orGTL3f</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Imported</v>
+        <v>Female</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>L8hy5JsqneC</v>
+        <v>bqoVhX2RfG4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Known Cluster</v>
+        <v>Male</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>C7gopCwNhoa</v>
+        <v>EVYKU2fIc6G</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Male</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Male</v>
+        <v>Unk Sex</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>EVYKU2fIc6G</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>MV</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>QLONA1SnwU5</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="C19" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <v>QRRRfUrxJs0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>≥ 85 y</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D20" s="4" t="str">
-        <v>GL19QsdIgIu</v>
+        <v>SZJNeRyrh22</v>
       </c>
     </row>
   </sheetData>
@@ -1319,13 +1337,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="88.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="104.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1338,7 +1356,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B2" s="4" t="str">
         <v>0-4 years</v>
@@ -1346,146 +1364,130 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>5-14 years</v>
+        <v>5-9 years</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>25-34 years</v>
+        <v>15-19 years</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>35-44 years</v>
+        <v>20-29 years</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>45-54 years</v>
+        <v>30-39 years</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>55-64 years</v>
+        <v>40-49 years</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>65-74 years</v>
+        <v>50-59 years</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>75-84 years</v>
+        <v>60-64 years</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Age in years (0-4, 5-14, 15-24, 25-34, 35-44, 45-54, 55-64, 65-74, 75-84, ≥ 85)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>≥ 85 years</v>
+        <v>65-69 years</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Female</v>
+        <v>70-74 years</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>Sex (Male/Female)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>Male</v>
+        <v>75-79 years</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>Imported</v>
+        <v>80+ years</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Age in years for COVID-19(0-4,5-9,10-14,15-19,20-29,30-39,40-49,50-59,60-64,65-69,70-74,75-79,80+,Unk)</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>Known Cluster</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Transmission Classification (Imported, Known Cluster, Community transmission, Unknown)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>Unknown Classification</v>
+        <v>Male</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="5" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B19" s="5" t="str">
-        <v>ECMO</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="str">
-        <v>Treatment Mode (Ventilation, ECMO, ICU)</v>
-      </c>
-      <c r="B20" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -1499,7 +1501,321 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Options</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Transmission Classification</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>No cases; Sporadic; Clusters; Community</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>UID</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Code</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Option set UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>NzPq5MlxCmh</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>Clusters</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>CLUSTERS</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>zUdhwKZdpT8</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Community</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>COMMUNITY</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>mF5r1p7sKcq</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>No cases</v>
+      </c>
+      <c r="C4" s="4" t="str">
+        <v>NO_CASES</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E4" s="4" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>AXl3Z9rLjLi</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>Sporadic</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <v>SPORADIC</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <v>QLANS0Gen0m</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
+    <col min="2" max="2" width="79.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Instruction</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>Left side</v>
+      </c>
+      <c r="D1" s="3" t="str">
+        <v>Operator</v>
+      </c>
+      <c r="E1" s="3" t="str">
+        <v>Right side</v>
+      </c>
+      <c r="F1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="G1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>New Cases hospitalised should be less than or equal to All new cases reported</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>New Cases hospitalised</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <v>All New Cases</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <v>bO8rXNzj0iR</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>Test with PCR should be less than or equal to tested</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>Tested with PCR</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <v>less_than_or_equal_to</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <v>Tested</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <v>gZwUbrTOa0g</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="C1" s="3" t="str">
+        <v>UID</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>2020-10-06</v>
+      </c>
+      <c r="C2" s="4" t="str">
+        <v>WY7h5pKok2I</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Validation Rule Group</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Validation Rule</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - PCR tests &lt;= tested</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>COVID-19</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>COVID19 - New Cases hospitalised &lt;= All New Cases</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1521,36 +1837,99 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19</v>
+        <v>COVID19</v>
       </c>
       <c r="B2" s="4" t="str">
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v>Property</v>
+      </c>
+      <c r="B1" s="3" t="str">
+        <v>Value</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v>Name:</v>
+      </c>
+      <c r="B2" s="4" t="str">
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v>Custom form:</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>No</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
+        <v>Sections:</v>
+      </c>
+      <c r="B4" s="4" t="str">
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="str">
+        <v>Last updated</v>
+      </c>
+      <c r="B5" s="5" t="str">
+        <v>2020-09-17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="str">
+        <v>UID:</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>uKtOZwDnIpM</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="153.7109375" customWidth="1"/>
-    <col min="7" max="7" width="42.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44.7109375" customWidth="1"/>
+    <col min="7" max="7" width="43.7109375" customWidth="1"/>
     <col min="8" max="8" width="25.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
     <col min="10" max="10" width="21.7109375" customWidth="1"/>
@@ -1590,16 +1969,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>zUcGi0Y384Y</v>
+        <v>ZTklbd8JtLn</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - Active cases</v>
+        <v>COVID19 - Active cases</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>Active cases</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v/>
+        <v>CV19_ACTIVE_CASES</v>
       </c>
       <c r="E2" s="4" t="str">
         <v/>
@@ -1614,94 +1993,94 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J2" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>kJoSHTinHGa</v>
+        <v>LeNVLm6SL1x</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - All cases</v>
+        <v>COVID19 - Case fatality rate (%)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>All cases</v>
+        <v>Case Fatality rate (%)</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE</v>
       </c>
       <c r="E3" s="5" t="str">
         <v/>
       </c>
       <c r="F3" s="5" t="str">
-        <v>All cases</v>
+        <v>Death (Confirmed + Probable)</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H3" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J3" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>dXAhOKiim1x</v>
+        <v>NP88sGFKpCQ</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - Case Fatality rate (%)</v>
+        <v>COVID19 - Case fatality rate among HW (%)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Case Fatality rate (%)</v>
+        <v>Case fatality rate HW (%)</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v/>
+        <v>CV19_CASE_FATALITY_RATE_HW</v>
       </c>
       <c r="E4" s="4" t="str">
         <v/>
       </c>
       <c r="F4" s="4" t="str">
-        <v>Deaths Reported</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="H4" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J4" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>fK1b7O6CuBV</v>
+        <v>VJHMO9gHkV5</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Cases treated by mechanical ventilation, ECMO or ICU</v>
+        <v>COVID19 - Closed cases</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Cases treated by type</v>
+        <v>Closed cases</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v/>
+        <v>CV19_CLOSED_CASES</v>
       </c>
       <c r="E5" s="5" t="str">
         <v/>
       </c>
       <c r="F5" s="5" t="str">
-        <v>Number of suspected cases that received mechanical ventilation, ECMO or admitted into intensive care unit</v>
+        <v>Closed cases</v>
       </c>
       <c r="G5" s="5" t="str">
         <v>1</v>
@@ -1710,30 +2089,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J5" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>S3Ty19GEaqn</v>
+        <v>TmKNBHtBx6D</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Closed cases</v>
+        <v>COVID19 - New Confirmed cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>Closed cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="E6" s="4" t="str">
         <v/>
       </c>
       <c r="F6" s="4" t="str">
-        <v>Active Cases</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G6" s="4" t="str">
         <v>1</v>
@@ -1742,30 +2121,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J6" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>ocBlGrHZy6Q</v>
+        <v>yzyWxXoSCny</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Confirmed cases</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="E7" s="5" t="str">
         <v/>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Suspected cases that were confirmed through laboratory testing (multiple lab tests may be conducted; this indicator assumes that the last test result).</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>1</v>
@@ -1774,30 +2153,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J7" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>zozhRzInMZm</v>
+        <v>U89bOzPbFyA</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by Transmission Classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="E8" s="4" t="str">
         <v/>
       </c>
       <c r="F8" s="4" t="str">
-        <v>Confirmed cases by Transmission Classification</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>1</v>
@@ -1806,30 +2185,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J8" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>r2VxAVW1IEy</v>
+        <v>DnleIypnqxJ</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - Deaths</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Deaths</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v/>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="E9" s="5" t="str">
         <v/>
       </c>
       <c r="F9" s="5" t="str">
-        <v>COVID-19 related deaths (deaths recorded among all suspected cases)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -1838,158 +2217,158 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J9" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>BmW2IAaxIBe</v>
+        <v>C6A59SObXV6</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - Hospitalised Cases</v>
+        <v>COVID19 - Positivity rate (%)</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Hospitalised Cases</v>
+        <v>Positivity rate (%)</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v/>
+        <v>CV19_POSITIVITY_RATE</v>
       </c>
       <c r="E10" s="4" t="str">
         <v/>
       </c>
       <c r="F10" s="4" t="str">
-        <v>Number of suspected or confirmed or probable cases that were admitted into hospital</v>
+        <v>New Confirmed cases</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>1</v>
+        <v>Tested</v>
       </c>
       <c r="H10" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J10" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>jHzx1zXeHzV</v>
+        <v>x6IelBioEX1</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Proportion of males among confirmed cases (%)</v>
+        <v>COVID19 - Proportion of HW amongst reported cases (%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Proportion of males among confirmed cases (%)</v>
+        <v>HW among confirmed cases (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v/>
+        <v>CV19_%_HW_AMONGST_REPORTED_CASES</v>
       </c>
       <c r="E11" s="5" t="str">
         <v/>
       </c>
       <c r="F11" s="5" t="str">
-        <v>Males among confirmed cases</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>Confirmed cases</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="H11" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="J11" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>UF7s1t1v6KG</v>
+        <v>cJZS7kSFFGl</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - Proportion of males among deaths(%)</v>
+        <v>COVID19 - Proportion of PCR tests (%)</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Proportion of males among deaths (%)</v>
+        <v>Proportion of PCR tests</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v/>
+        <v>CV19_%_PCR_TESTS</v>
       </c>
       <c r="E12" s="4" t="str">
         <v/>
       </c>
       <c r="F12" s="4" t="str">
-        <v>Males among deaths</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>Deaths</v>
+        <v>Tested</v>
       </c>
       <c r="H12" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J12" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>gYt2GEAdCJK</v>
+        <v>K2JqazsxhvP</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Recovery rate (%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Recovery rate (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v/>
+        <v>CV19_RECOVERY_RATE</v>
       </c>
       <c r="E13" s="5" t="str">
         <v/>
       </c>
       <c r="F13" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>All cases (Confirmed + Probable)</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="J13" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>JpRDu51rbg5</v>
+        <v>pxqFjCNLkzD</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v/>
+        <v>CV19_TESTED</v>
       </c>
       <c r="E14" s="4" t="str">
         <v/>
       </c>
       <c r="F14" s="4" t="str">
-        <v>Transmission pattern (Community cases)</v>
+        <v>Tested</v>
       </c>
       <c r="G14" s="4" t="str">
         <v>1</v>
@@ -1998,30 +2377,30 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J14" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>vECy4BgZqRF</v>
+        <v>jgyO0rV708H</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (No cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v/>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="E15" s="5" t="str">
         <v/>
       </c>
       <c r="F15" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="G15" s="5" t="str">
         <v>1</v>
@@ -2030,113 +2409,17 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="J15" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>GszrLGBvHhg</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>COVID-19 - Provinces/regions with Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="G16" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>PkGdfHQyWWH</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>COVID-19 - Recovered cases</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>Recovered cases</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v/>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>Number of cases that are recovered.</v>
-      </c>
-      <c r="G17" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I17" s="5" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J17" s="5" t="str">
-        <v>YKyPfpFUAVo</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>dsho3rAaUkr</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>COVID-19 - Recovery rate (%)</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>Case Recovery rate</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v/>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>Cases Recovered</v>
-      </c>
-      <c r="G18" s="4" t="str">
-        <v>All suspected cases (Confirmed+Probable)</v>
-      </c>
-      <c r="H18" s="4" t="str">
-        <v>Percentage</v>
-      </c>
-      <c r="I18" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="J18" s="4" t="str">
-        <v>YKyPfpFUAVo</v>
+        <v>UGXgY58CxjG</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2171,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2018-01-16</v>
+        <v>2020-09-09</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>kHy61PbChXr</v>
@@ -2195,14 +2478,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -2220,29 +2503,29 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>04. COVID-19 Surveillance (Aggregate)</v>
+        <v>COVID19 - Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" customWidth="1"/>
+    <col min="3" max="3" width="93.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" customWidth="1"/>
@@ -2270,356 +2553,236 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>ud3dbLWVafm</v>
+        <v>jTGq07MlmMp</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Chart</v>
+        <v>Pivot table</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>ZcYLgBQrhgu</v>
+        <v>btrkVNdRwnO</v>
       </c>
       <c r="E2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>n2mZrxngMFR</v>
+        <v>oaBx9hR7FFR</v>
       </c>
       <c r="B3" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>nIVBxZaZ8Gd</v>
+        <v>jmn7HoMmBHC</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>FjfJIiULctQ</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
       <c r="B4" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>lIAZDq6H4dF</v>
+        <v>JNHOYQEIN3V</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
       <c r="B5" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>o9HS22p81W0</v>
+        <v>P7syfXG9dNm</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>E6w4iwPkaRM</v>
       </c>
       <c r="B6" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>YzYCsOsZDz2</v>
+        <v>IeZQZcgmAfV</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>AwrThZVBW5g</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Chart</v>
+        <v>Map</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>dFmHVADG2t5</v>
+        <v>KWM5EsM8hYR</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>WcRHBfw09Iq</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>cSmHf59IIs5</v>
+        <v>qTkvVnIP5Ri</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E94X1H21okK</v>
       </c>
       <c r="B9" s="5" t="str">
         <v>Chart</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>kz9Z0mKZQbN</v>
+        <v>KMsy5gLLUWr</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>neIuzgRUO0N</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Map</v>
+        <v>Chart</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>hoZsDsseA6B</v>
+        <v>JZ4Jt9JxsVh</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>p6zlpJrZzJV</v>
+        <v>pQ6jw6r59Op</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Pivot table</v>
+        <v>Chart</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>kQCzFsC1eEU</v>
+        <v>YocjDGUCP18</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>cTcbZ8ht1zi</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
       <c r="B12" s="4" t="str">
         <v>Chart</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>r83aoS5wveR</v>
+        <v>dbn6GloPaRP</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>GjZAEBGomjW</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>KYC90zR9e6n</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>VvJv2JhRgLE</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>h0FivHWebim</v>
-      </c>
-      <c r="E15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F15" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="str">
-        <v>HrI5yNYmham</v>
-      </c>
-      <c r="B16" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C16" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
-      </c>
-      <c r="D16" s="4" t="str">
-        <v>GvYhMDZrNH9</v>
-      </c>
-      <c r="E16" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F16" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
-      </c>
-      <c r="B17" s="5" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <v>hOLM46Ckolu</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <v>BRV6jGG6Oxl</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="str">
-        <v>WSZu4jpViok</v>
-      </c>
-      <c r="B18" s="4" t="str">
-        <v>Chart</v>
-      </c>
-      <c r="C18" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
-      </c>
-      <c r="D18" s="4" t="str">
-        <v>NMmB1l6X07Y</v>
-      </c>
-      <c r="E18" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="F18" s="4" t="str">
-        <v>BRV6jGG6Oxl</v>
+        <v>GdRQEdWJEMH</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="93.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2641,281 +2804,142 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Active and Closed Cases last 14 days</v>
+        <v>COVID19 - Active and Closed Cases last 12 weeks</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>WJ8cY4u7vgZ</v>
+        <v>Sf2KIcQRyMj</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v xml:space="preserve">COVID-19 - All cumulative confirmed cases by Transmission Classification -  </v>
+        <v>COVID19 - Case recovery and fatality rates last 12 weeks</v>
       </c>
       <c r="B3" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>KYC90zR9e6n</v>
+        <v>pQ6jw6r59Op</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - Case Recovery and Fatality Rates last 14 days</v>
+        <v>COVID19 - Closed and active cases at subnational last months</v>
       </c>
       <c r="B4" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>HrI5yNYmham</v>
+        <v>neIuzgRUO0N</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - Closed and Active Cases at subnational Last 14 days</v>
+        <v>COVID19 - Confirmed cases by sex in the last 14 weeks</v>
       </c>
       <c r="B5" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>lRccab7cjgV</v>
+        <v>E94X1H21okK</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases at subnational by Sex This and Last 12 Weeks</v>
+        <v xml:space="preserve">COVID19 - Cumulative tests conducted, cases reported, hospitalised, discharged and deaths  </v>
       </c>
       <c r="B6" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>MUWm0tv2W5z</v>
+        <v>E6w4iwPkaRM</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - Confirmed Cases by Age group last 14 days</v>
+        <v>COVID19 - Deaths by age groups last weeks</v>
       </c>
       <c r="B7" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>IB4zviSI7Y6</v>
+        <v>WcRHBfw09Iq</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - Confirmed Cases LAST 14 DAYS</v>
+        <v>COVID19 - Fatality rate amongst HW</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>WSZu4jpViok</v>
+        <v>BGGBmj9Yuu7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Cumulative Cases Reported, Tested, Hospitalised and Deaths - Todate</v>
+        <v>COVID19 - HW amongst reported cases this year</v>
       </c>
       <c r="B9" s="5" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>b0kD0pUzIkI</v>
+        <v>oaBx9hR7FFR</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Cumulative confirmed cases among males</v>
+        <v>COVID19 - New confirmed cases and deaths in the last 12 weeks</v>
       </c>
       <c r="B10" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>FjfJIiULctQ</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="5" t="str">
-        <v>COVID-19 - Cumulative deaths among males</v>
-      </c>
-      <c r="B11" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>n2mZrxngMFR</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="str">
-        <v>COVID-19 - Deaths among  males by Age Groups last 14 days</v>
-      </c>
-      <c r="B12" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>ud3dbLWVafm</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Deaths by Age Groups last 14 days</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>cTcbZ8ht1zi</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Modes of Treatment - This Month</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>zfM9c4Zg59D</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="str">
-        <v>COVID-19 - Provinces/regions and Transmission patterns  last 4 weeks</v>
-      </c>
-      <c r="B15" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <v>WY2HxfVvgF8</v>
+        <v>eha82bnB8N1</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="3" t="str">
-        <v>Name</v>
-      </c>
-      <c r="B1" s="3" t="str">
-        <v>Custom form</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Sections</v>
-      </c>
-      <c r="D1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>UID</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B2" s="4" t="str">
-        <v>No</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>kIfMNugiTgd</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>No</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>Yes</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>Vs7Bd0pHjS9</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" width="81.7109375" customWidth="1"/>
+    <col min="1" max="1" width="85.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -2937,37 +2961,23 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v xml:space="preserve">COVID-19 - Cumulative all cases, confirmed, recovered and death by sex and age </v>
+        <v>COVID19 - Tested, tests with PCR and positivity rate by subnational level this year</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>p6zlpJrZzJV</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 - Recovery and fatality rate by sex and age - This Month</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>RncWJdNUuJ9</v>
+        <v>jTGq07MlmMp</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2996,30 +3006,30 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID 19 - Confirmed cases by subnational This week</v>
+        <v>COVID19 - Cumulative confirmed cases by subnational</v>
       </c>
       <c r="B2" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-05</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>rFwk97WsyWV</v>
+        <v>AwrThZVBW5g</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3040,7 +3050,7 @@
         <v>COVID19 access</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-04-24</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>DoYehxUvmwT</v>
@@ -3051,28 +3061,17 @@
         <v>COVID19 admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-21</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>w4iJeNKy9br</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID19 data capture</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>k8Fk0kuhOeK</v>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3097,13 +3096,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>who</v>
+        <v>covid19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2018-07-13</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>vUeLeQMSwhN</v>
+        <v>F0YhCM0Pi73</v>
       </c>
     </row>
   </sheetData>
@@ -3112,99 +3111,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Section name</v>
+        <v>Last updated</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>Last updated</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>COVID-19 Surveillance (Aggregate)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>COVID-19 Weekly Provincial Report</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>BF8373CGyyT</v>
+        <v>i9rpQqB3Hfh</v>
       </c>
     </row>
   </sheetData>
@@ -3213,254 +3149,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="77.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>Data Set</v>
+        <v>Data Set Section</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>Data Set Section</v>
-      </c>
-      <c r="C1" s="3" t="str">
-        <v>Section UID</v>
-      </c>
-      <c r="D1" s="3" t="str">
         <v>Data Element</v>
-      </c>
-      <c r="E1" s="3" t="str">
-        <v>Data Element UID</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C2" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D3" s="5" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
-      </c>
-      <c r="E3" s="5" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Cases and Deaths Reported by Age and Gender</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>xcjauPeiVnT</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>Cases Tested and Hospitalised</v>
-      </c>
-      <c r="C7" s="5" t="str">
-        <v>DalHE1qVrX5</v>
-      </c>
-      <c r="D7" s="5" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
-      </c>
-      <c r="E7" s="5" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New cases treated</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <v>vTJZ2dOf97q</v>
-      </c>
-      <c r="D8" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-      <c r="E8" s="4" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C9" s="5" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D9" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
-      </c>
-      <c r="E9" s="5" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>Transmission classification</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Transmission classification</v>
-      </c>
-      <c r="C10" s="4" t="str">
-        <v>pjQjc8NdZb8</v>
-      </c>
-      <c r="D10" s="4" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
-      </c>
-      <c r="E10" s="4" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="E11" s="5" t="str">
-        <v>njg6PAh5gw6</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
+        <v>Aggregate Weekly Surveillance</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C12" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
-      </c>
-      <c r="E12" s="4" t="str">
-        <v>e1xTRwfWega</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>h34jPNnKkJK</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern of the province/state this week (Mark all the applies)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>BF8373CGyyT</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>RC7RG6mexD2</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
   </sheetData>
@@ -3469,16 +3260,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
@@ -3508,13 +3299,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>COVID-19 - Cases tested</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Cases tested</v>
+        <v>New Cases Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>COVID_19_CASES_TESTED</v>
+        <v>CV19_NEW_CONF_PROB_HW_CASES</v>
       </c>
       <c r="D2" s="4" t="str">
         <v/>
@@ -3523,136 +3314,136 @@
         <v>default</v>
       </c>
       <c r="F2" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>kX2J7E3H3YO</v>
+        <v>SU1j9CmCuW9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Confirmed cases by transmission classification</v>
+        <v>New Confirmed Cases</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>COVID_19_CONFIRMED_CASES_BY_TC</v>
+        <v>CV19_NEW_CONF_CASES</v>
       </c>
       <c r="D3" s="5" t="str">
         <v/>
       </c>
       <c r="E3" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>zh8QqfZJqx4</v>
+        <v>bmbNyNoJcXP</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>New cases hospitalised</v>
+        <v>New Confirmed Deaths</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>COVID_19_NEW_CASES_HOSPITALISED</v>
+        <v>CV19_NEW_CONF_DEATHS</v>
       </c>
       <c r="D4" s="4" t="str">
         <v/>
       </c>
       <c r="E4" s="4" t="str">
-        <v>default</v>
+        <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>pwMpWi75Z6T</v>
+        <v>rBw83gVQLHK</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>COVID-19 - New cases treated</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>New cases treated</v>
+        <v>New Deaths Among HW (Confirmed + Probable)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>COVID_19_NEW_CASES_TREATED</v>
+        <v>CV19_NEW_CONF_PROB_HW_DEATHS</v>
       </c>
       <c r="D5" s="5" t="str">
         <v/>
       </c>
       <c r="E5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F5" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-10-06</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>bVLbViCg2Zw</v>
+        <v>DI9JgEJ3t8v</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>New confirmed cases (sex/age)</v>
+        <v>New Discharged Cases</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>COVID_19_NEW_CONFIRMED_CASES</v>
+        <v>CV19_NEW_CONF_PROB_DISCHARGED</v>
       </c>
       <c r="D6" s="4" t="str">
         <v/>
       </c>
       <c r="E6" s="4" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>CnPsS2xE8UN</v>
+        <v>fJ7Qi1zcdAR</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>New deaths (sex/age)</v>
+        <v>New Hospitalized Cases</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>COVID_19_NEW_DEATHS</v>
+        <v>CV19_NEW_CONF_PROB_HOSPITALIZED</v>
       </c>
       <c r="D7" s="5" t="str">
         <v/>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Age and sex (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>BkH5UYzo3SM</v>
+        <v>cW0odY9vhrd</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>New Suspected cases (sex/age)</v>
+        <v>New Probable Cases</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>COVID_19_NEW_SUSPECTED_CASES</v>
+        <v>CV19_NEW_PROB_CASES</v>
       </c>
       <c r="D8" s="4" t="str">
         <v/>
@@ -3661,21 +3452,21 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>MpYJAYuLpim</v>
+        <v>VnkErE22ELJ</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>Recovered cases (sex/age)</v>
+        <v>New Probable Deaths</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>COVID_19_RECOVERED_CASES</v>
+        <v>CV19_NEW_PROB_DEATHS</v>
       </c>
       <c r="D9" s="5" t="str">
         <v/>
@@ -3684,44 +3475,44 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>2020-03-19</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G9" s="5" t="str">
-        <v>rvYTAOrBrtY</v>
+        <v>N59eghaBpM7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - Tested</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>Suspected cases by transmission classification</v>
+        <v>Tested</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>COVID_19_SUSPECTED_CASES_BY_TC</v>
+        <v>CV19_TESTED</v>
       </c>
       <c r="D10" s="4" t="str">
         <v/>
       </c>
       <c r="E10" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
+        <v>default</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>hwLQyZKeD0E</v>
+        <v>E1pXvzyZzKB</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>Transmission pattern (Cluster cases)</v>
+        <v>Tested with PCR Assay</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>COVID_19_TP_CLUSTER_CASES</v>
+        <v>CV19_TESTED_PCR</v>
       </c>
       <c r="D11" s="5" t="str">
         <v/>
@@ -3730,21 +3521,21 @@
         <v>default</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>e1xTRwfWega</v>
+        <v>pZtyMNtYPLM</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>Transmission pattern (Community  cases)</v>
+        <v>Transmission Classification</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>COVID_19_TP_COMMUNITY_CASES</v>
+        <v>CV19_TRANS_CLASS</v>
       </c>
       <c r="D12" s="4" t="str">
         <v/>
@@ -3753,56 +3544,10 @@
         <v>default</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>RC7RG6mexD2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>Transmission pattern (No cases)</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <v>COVID_19_TP_NO_CASES</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <v/>
-      </c>
-      <c r="E13" s="5" t="str">
-        <v>default</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <v>njg6PAh5gw6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>Transmission pattern (Sporadic cases)</v>
-      </c>
-      <c r="C14" s="4" t="str">
-        <v>COVID_19_TP_SPORADIC_CASES</v>
-      </c>
-      <c r="D14" s="4" t="str">
-        <v/>
-      </c>
-      <c r="E14" s="4" t="str">
-        <v>default</v>
-      </c>
-      <c r="F14" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="G14" s="4" t="str">
-        <v>h34jPNnKkJK</v>
+        <v>sWCFbUawFDa</v>
       </c>
     </row>
   </sheetData>
@@ -3811,13 +3556,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3833,7 +3578,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>COVID-19 - New Suspected cases (sex/age)</v>
+        <v>COVID19 - Transmission Classification</v>
       </c>
     </row>
     <row r="3">
@@ -3841,7 +3586,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>COVID-19 - Recovered cases (sex/age)</v>
+        <v>COVID19 - New Confirmed Cases</v>
       </c>
     </row>
     <row r="4">
@@ -3849,7 +3594,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>COVID-19 - New deaths (sex/age)</v>
+        <v>COVID19 - New Confirmed Deaths</v>
       </c>
     </row>
     <row r="5">
@@ -3857,7 +3602,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>COVID-19 - Transmission pattern (Sporadic cases)</v>
+        <v>COVID19 - New Probable Cases</v>
       </c>
     </row>
     <row r="6">
@@ -3865,7 +3610,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Cluster cases)</v>
+        <v>COVID19 - Tested with PCR Assay</v>
       </c>
     </row>
     <row r="7">
@@ -3873,7 +3618,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVID-19 - Suspected cases by transmission classification</v>
+        <v>COVID19 - New Probable Deaths</v>
       </c>
     </row>
     <row r="8">
@@ -3881,7 +3626,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (Community cases)</v>
+        <v>COVID19 - Tested</v>
       </c>
     </row>
     <row r="9">
@@ -3889,7 +3634,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>COVID-19 - New confirmed cases (sex/age)</v>
+        <v>COVID19 - New Hospitalized Cases</v>
       </c>
     </row>
     <row r="10">
@@ -3897,7 +3642,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>COVID-19 - New cases hospitalised</v>
+        <v>COVID19 - New Cases Among HW (Confirmed + Probable)</v>
       </c>
     </row>
     <row r="11">
@@ -3905,7 +3650,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>COVID-19 - Confirmed cases by transmission classification</v>
+        <v>COVID19 - New Discharged Cases</v>
       </c>
     </row>
     <row r="12">
@@ -3913,23 +3658,7 @@
         <v>COVID-19</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>COVID-19 - New cases treated</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B13" s="5" t="str">
-        <v>COVID-19 - Cases tested</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="str">
-        <v>COVID-19</v>
-      </c>
-      <c r="B14" s="4" t="str">
-        <v>COVID-19 - Transmission pattern (No cases)</v>
+        <v>COVID19 - New Deaths Among HW (Confirmed + Probable)</v>
       </c>
     </row>
   </sheetData>
@@ -3938,15 +3667,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3968,13 +3697,13 @@
         <v>Age and sex (COVID-19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>o3OiZXHwBzY</v>
+        <v>UPxdJOxz2I7</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Age (COVID-19); Sex</v>
+        <v>Age (COVID19); Sex (with unknown)</v>
       </c>
     </row>
     <row r="3">
@@ -3982,41 +3711,13 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2017-05-28</v>
+        <v>2020-05-11</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>bjDvmb4bfuf</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>default</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>2020-03-19</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <v>FGDN1aBqJnt</v>
-      </c>
-      <c r="D4" s="4" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>sRwqVdFcBat</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Treatment Type (COVID-19)</v>
       </c>
     </row>
   </sheetData>
@@ -4025,15 +3726,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="126.7109375" customWidth="1"/>
+    <col min="4" max="4" width="176.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4052,16 +3753,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Age (COVID-19)</v>
+        <v>Age (COVID19)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-06</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>prZlmHqhxLO</v>
+        <v>RrZWSJ6CsLs</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>0-4 years; 5-14 years; 15-24 years; 25-34 years; 35-44 years; 45-54 years; 55-64 years; 65-74 years; 75-84 years; ≥ 85 years</v>
+        <v>0-4 years; 5-9 years; 10-14 years; 15-19 years; 20-29 years; 30-39 years; 40-49 years; 50-59 years; 60-64 years; 65-69 years; 70-74 years; 75-79 years; 80+ years; Unknown age</v>
       </c>
     </row>
     <row r="3">
@@ -4069,7 +3770,7 @@
         <v>default</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-26</v>
+        <v>2020-10-12</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>GLevLNI9wkl</v>
@@ -4080,44 +3781,16 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Sex</v>
+        <v>Sex (with unknown)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-26</v>
+        <v>2020-09-22</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>FRwO58KwwJt</v>
+        <v>b7peexUktxt</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Male; Female</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="str">
-        <v>Transmission Classification (COVID-19)</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C5" s="5" t="str">
-        <v>v1atVR1HnCr</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <v>Imported; Known Cluster; Community transmission; Unknown Classification</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="str">
-        <v>Treatment Type (COVID-19)</v>
-      </c>
-      <c r="B6" s="4" t="str">
-        <v>2020-03-26</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <v>PWWzA79GcCG</v>
-      </c>
-      <c r="D6" s="4" t="str">
-        <v>Mechanical ventilation; ECMO; Admitted in intensive care unit (ICU)</v>
+        <v>Male; Female; Unknown Sex</v>
       </c>
     </row>
   </sheetData>
@@ -4126,12 +3799,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
@@ -4149,13 +3822,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>0-1 years</v>
+        <v>0-14 years</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2019-07-03</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>uueCp2RIGCJ</v>
+        <v>IoqDBYr0rH5</v>
       </c>
     </row>
     <row r="3">
@@ -4163,7 +3836,7 @@
         <v>0-4 years</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>UPvKbcqTEY3</v>
@@ -4171,255 +3844,189 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>15-24 years</v>
+        <v>10-14 years</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>ls9vGYWbvwG</v>
+        <v>ftXCKvbuGgj</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>15-49 years</v>
+        <v>15-19 years</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>jqg45gLQRYI</v>
+        <v>dENFBee17Oi</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>2-4 years</v>
+        <v>20-29 years</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>jxOEQ4Ss4bM</v>
+        <v>GERCWxK3mvz</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>25-34 years</v>
+        <v>30-39 years</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>O6UJSfL4psp</v>
+        <v>bY3NyagrzeD</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>35-44 years</v>
+        <v>40-49 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>utyLRFta4ie</v>
+        <v>tTmsWzvoEUv</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>45-54 years</v>
+        <v>5-9 years</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>nkQw9lhkbGV</v>
+        <v>J205eXYNH7q</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>5-14 years</v>
+        <v>50-59 years</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>pa0cY66MrG6</v>
+        <v>BOCPEdURsYX</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>50-64 years</v>
+        <v>60-64 years</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Yl34dHOPpZ0</v>
+        <v>TEBfAmuOSJk</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>55-64 years</v>
+        <v>65-69 years</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Lo1gxiS8zap</v>
+        <v>gHA96noC0iO</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>65-74 years</v>
+        <v>70-74 years</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>AlUYlzoMVvN</v>
+        <v>Po7T5dd3tQs</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>65-79 years</v>
+        <v>75-79 years</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>ZPzdstvH08a</v>
+        <v>xWXUBYNycnE</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>75-84 years</v>
+        <v>80+ years</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>2020-03-25</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>R4m7KraS4aZ</v>
+        <v>c2hLbh0drQI</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>Admitted in intensive care unit (ICU)</v>
+        <v>default</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2018-05-30</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>zUAhtH6iiyz</v>
+        <v>xYerKDKCefk</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>Community transmission</v>
+        <v>Female</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>hH4LYNplIeA</v>
+        <v>FFA9e1yIXCT</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>default</v>
+        <v>Male</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>2018-05-30</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>xYerKDKCefk</v>
+        <v>MP15bHaQh2x</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>ECMO</v>
+        <v>Unknown age</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>mg1cBsgdqHC</v>
+        <v>WNPpyVkVaL3</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>Female</v>
+        <v>Unknown Sex</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>2020-03-18</v>
+        <v>2020-09-17</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>FFA9e1yIXCT</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="5" t="str">
-        <v>Imported</v>
-      </c>
-      <c r="B21" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C21" s="5" t="str">
-        <v>y8TxHRrY1eN</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="str">
-        <v>Known Cluster</v>
-      </c>
-      <c r="B22" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C22" s="4" t="str">
-        <v>LIRv9sIHNOD</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="5" t="str">
-        <v>Male</v>
-      </c>
-      <c r="B23" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C23" s="5" t="str">
-        <v>MP15bHaQh2x</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="str">
-        <v>Mechanical ventilation</v>
-      </c>
-      <c r="B24" s="4" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C24" s="4" t="str">
-        <v>qoxRSWYj9cB</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="5" t="str">
-        <v>Unknown Classification</v>
-      </c>
-      <c r="B25" s="5" t="str">
-        <v>2020-03-18</v>
-      </c>
-      <c r="C25" s="5" t="str">
-        <v>YfLFBoAcjE2</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="str">
-        <v>≥ 85 years</v>
-      </c>
-      <c r="B26" s="4" t="str">
-        <v>2020-03-25</v>
-      </c>
-      <c r="C26" s="4" t="str">
-        <v>F3RlEj6nnR3</v>
+        <v>kuP5EmQRFke</v>
       </c>
     </row>
   </sheetData>

</xml_diff>